<commit_message>
New: Field SheetChannelBuilder.name is now validated to comply with channel name restrictions
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -11,12 +11,289 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>mU$ed)uPodo*Lyi</t>
+  </si>
+  <si>
+    <t>download path</t>
+  </si>
+  <si>
+    <t>downloads</t>
+  </si>
+  <si>
+    <t>download max size</t>
+  </si>
+  <si>
+    <t>// About 8MB</t>
+  </si>
   <si>
     <t>info</t>
   </si>
   <si>
     <t>Initialized Narrator, configuring now</t>
+  </si>
+  <si>
+    <t>prepare save</t>
+  </si>
+  <si>
+    <t>narrator.save</t>
+  </si>
+  <si>
+    <t>configure story service</t>
+  </si>
+  <si>
+    <t>stories</t>
+  </si>
+  <si>
+    <t>monitored channels</t>
+  </si>
+  <si>
+    <t>admin/test</t>
+  </si>
+  <si>
+    <t>moderator/mods-room</t>
+  </si>
+  <si>
+    <t>discordia/control</t>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>@narrator</t>
+  </si>
+  <si>
+    <t>story category</t>
+  </si>
+  <si>
+    <t>Narrator</t>
+  </si>
+  <si>
+    <t>story bots</t>
+  </si>
+  <si>
+    <t>StoryBot #1</t>
+  </si>
+  <si>
+    <t>NjgyNzg3NDcxNjk5ODY5Njk2.XliJwg.FbHRYJvuVMQxd7oesNe9WxWfo-w</t>
+  </si>
+  <si>
+    <t>StoryBot #2</t>
+  </si>
+  <si>
+    <t>NjgyNzg5NjQyNTgzNDA4Njcz.XliJ2Q.JcbF-iO_KTNSKtF64jZehNF2BrU</t>
+  </si>
+  <si>
+    <t>StoryBot #3</t>
+  </si>
+  <si>
+    <t>NjgyNzkwMTUwNjIyNjc1MDc1.XliJ5A.9h68c7A3CQIhqwculzux5cjgjsk</t>
+  </si>
+  <si>
+    <t>StoryBot #4</t>
+  </si>
+  <si>
+    <t>NjgyNzkxMTAwMjgwMzQwNTEw.XliJ7Q.zKRHQtTA0ew7mQiV5Iq0G8ps0bc</t>
+  </si>
+  <si>
+    <t>StoryBot #5</t>
+  </si>
+  <si>
+    <t>NjgyNzkxNDAyNTY4Mjg2MjM5.XliJ-A.mW2tHnkgTiEDTsmwhy9odNkGYwA</t>
+  </si>
+  <si>
+    <t>story bot timeout</t>
+  </si>
+  <si>
+    <t>15 mins</t>
+  </si>
+  <si>
+    <t>story bot typing interval</t>
+  </si>
+  <si>
+    <t>7s</t>
+  </si>
+  <si>
+    <t>story channel timestep</t>
+  </si>
+  <si>
+    <t>100ms</t>
+  </si>
+  <si>
+    <t>story reply selection delay</t>
+  </si>
+  <si>
+    <t>1.5s</t>
+  </si>
+  <si>
+    <t>upload acknowledge message</t>
+  </si>
+  <si>
+    <t>&lt;embed</t>
+  </si>
+  <si>
+    <t>000000</t>
+  </si>
+  <si>
+    <t>Alright %(sender), let me look at your story.</t>
+  </si>
+  <si>
+    <t>Okay, okay %(sender), i'm downloading your story now.</t>
+  </si>
+  <si>
+    <t>upload unknown error</t>
+  </si>
+  <si>
+    <t>Derp derpity derp derp error!</t>
+  </si>
+  <si>
+    <t>Oops! Everything borked!</t>
+  </si>
+  <si>
+    <t>upload error message</t>
+  </si>
+  <si>
+    <t>FF7E7E</t>
+  </si>
+  <si>
+    <t>ZZzzt %(sender), I can't make sense of this... Ask Azmi for help!
+Here's a more detailed explanation:
+```
+%(error)
+```</t>
+  </si>
+  <si>
+    <t>CRASH! %(sender), I crashed pretty hard right there... Azk Azmi for Zhelp!
+Here's the precise reason why:
+```
+%(error)
+```</t>
+  </si>
+  <si>
+    <t>upload success message</t>
+  </si>
+  <si>
+    <t>%(sender) Cool!, I've looked at your story and I think its... o.. k.... To play, ping me with this story code:
+```
+@Narrator %(code)
+```</t>
+  </si>
+  <si>
+    <t>%(sender) That... was... amazing!, I'm sure others would agree too!. To play, ping me with this story code:
+```
+@Narrator %(code)
+```</t>
+  </si>
+  <si>
+    <t>story not found message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorry %(sender), I cant find Story #%(code)... </t>
+  </si>
+  <si>
+    <t>Are you okay %(sender)?, There is no Story #%(code) !</t>
+  </si>
+  <si>
+    <t>intro</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>`%(title)`</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>by %(author)
+%(description)
+Choose your character:</t>
+  </si>
+  <si>
+    <t>player waiting</t>
+  </si>
+  <si>
+    <t>%(choiceEmote) **`%(name)`**
+`... waiting for player ...`</t>
+  </si>
+  <si>
+    <t>player joined</t>
+  </si>
+  <si>
+    <t>%(choiceEmote) **`%(name)`**
+%(player) %(description)</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>preparing</t>
+  </si>
+  <si>
+    <t>%(:yes:) Getting ready...</t>
+  </si>
+  <si>
+    <t>not enough resources</t>
+  </si>
+  <si>
+    <t>%(:no:) Sorry, not enough resources to start this story. Try again later!</t>
+  </si>
+  <si>
+    <t>starting</t>
+  </si>
+  <si>
+    <t>%(:yes:) Starting now...</t>
+  </si>
+  <si>
+    <t>waiting color</t>
+  </si>
+  <si>
+    <t>preparing color</t>
+  </si>
+  <si>
+    <t>0088FF</t>
+  </si>
+  <si>
+    <t>not enough resources color</t>
+  </si>
+  <si>
+    <t>starting color</t>
+  </si>
+  <si>
+    <t>80FF7F</t>
+  </si>
+  <si>
+    <t>intro invite timeout</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>intro concluded timeout</t>
+  </si>
+  <si>
+    <t>3 min</t>
+  </si>
+  <si>
+    <t>instance timeout</t>
+  </si>
+  <si>
+    <t>choose reply message</t>
+  </si>
+  <si>
+    <t>%(player) Choose your reply:
+%(selection)</t>
+  </si>
+  <si>
+    <t>choose reply row format</t>
+  </si>
+  <si>
+    <t>%(choiceEmote) %(message)</t>
   </si>
   <si>
     <t>Added all services</t>
@@ -77,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -85,11 +362,20 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -144,10 +430,10 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -171,11 +457,10 @@
       <c r="Y2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -198,11 +483,14 @@
       <c r="Y3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -225,11 +513,18 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4">
+        <f>8 * 1000 * 1000</f>
+        <v>8000000</v>
+      </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -252,15 +547,10 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -283,11 +573,10 @@
       <c r="Y6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -310,19 +599,10 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4">
-        <v>5000.0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -345,11 +625,14 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -399,11 +682,16 @@
       <c r="Y10" s="1"/>
     </row>
     <row r="11">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4">
+        <v>100.0</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -480,12 +768,20 @@
       <c r="Y13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="1"/>
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1000.0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>9999.0</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -507,12 +803,12 @@
       <c r="Y14" s="1"/>
     </row>
     <row r="15">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -534,12 +830,15 @@
       <c r="Y15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -566,7 +865,9 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -593,7 +894,9 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -645,10 +948,14 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="F20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="4"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -699,9 +1006,13 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -753,11 +1064,16 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="D24" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="F24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -782,9 +1098,12 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="F25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -809,9 +1128,12 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="F26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -836,9 +1158,12 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="F27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -863,9 +1188,12 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="F28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -915,9 +1243,13 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="D30" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="F30" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -942,10 +1274,14 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="D31" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="G31" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -969,10 +1305,14 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="D32" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="G32" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -996,10 +1336,14 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="D33" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="G33" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1050,12 +1394,20 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="D35" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="G35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1080,9 +1432,15 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="G36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1131,11 +1489,13 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="D38" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
+      <c r="G38" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -1160,9 +1520,9 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="G39" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -1188,7 +1548,6 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -1212,16 +1571,19 @@
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="D41" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
+      <c r="G41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -1241,14 +1603,8 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="4"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -1268,14 +1624,8 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="4"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -1295,14 +1645,8 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="4"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -1322,14 +1666,8 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="4"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
@@ -1349,14 +1687,15 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
+      <c r="G46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
@@ -1376,14 +1715,8 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="4"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
@@ -1403,14 +1736,8 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="4"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
@@ -1430,14 +1757,8 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="4"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
@@ -1457,14 +1778,8 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="4"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
@@ -1484,10 +1799,9 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -1509,16 +1823,13 @@
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
+      <c r="D52" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
+      <c r="G52" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
@@ -1539,13 +1850,6 @@
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
@@ -1566,13 +1870,6 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
@@ -1593,13 +1890,6 @@
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
@@ -1620,13 +1910,6 @@
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
@@ -1647,13 +1930,9 @@
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
+      <c r="G57" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
@@ -1674,13 +1953,6 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
@@ -1701,13 +1973,6 @@
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
@@ -1728,13 +1993,6 @@
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
@@ -1755,13 +2013,6 @@
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
@@ -1782,9 +2033,6 @@
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -1806,12 +2054,19 @@
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
+      <c r="D63" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
+      <c r="G63" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
@@ -1835,10 +2090,15 @@
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
+      <c r="G64" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
@@ -1863,9 +2123,6 @@
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -1887,9 +2144,15 @@
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
+      <c r="D66" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -1915,13 +2178,12 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
+      <c r="E67" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
@@ -1943,12 +2205,6 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
@@ -1970,12 +2226,6 @@
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
@@ -1997,12 +2247,6 @@
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
@@ -2024,12 +2268,6 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
@@ -2050,14 +2288,13 @@
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
+      <c r="E72" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F72" s="2"/>
+      <c r="G72" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
@@ -2077,14 +2314,8 @@
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
@@ -2104,14 +2335,8 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
@@ -2131,14 +2356,13 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
+      <c r="E75" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F75" s="2"/>
+      <c r="G75" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
@@ -2158,14 +2382,8 @@
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
@@ -2185,14 +2403,8 @@
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
@@ -2212,9 +2424,15 @@
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
+      <c r="E78" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
@@ -2240,9 +2458,13 @@
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
+      <c r="F79" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
+      <c r="H79" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
@@ -2267,8 +2489,12 @@
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
+      <c r="F80" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
@@ -2294,10 +2520,13 @@
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
+      <c r="F81" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
+      <c r="I81" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
@@ -2321,10 +2550,13 @@
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
+      <c r="F82" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
+      <c r="I82" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
@@ -2348,10 +2580,13 @@
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
+      <c r="F83" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
+      <c r="I83" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
@@ -2375,10 +2610,13 @@
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
+      <c r="F84" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
+      <c r="I84" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
@@ -2427,14 +2665,18 @@
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
+      <c r="D86" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
+      <c r="F86" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="7"/>
+      <c r="K86" s="7"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
@@ -2454,14 +2696,18 @@
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
+      <c r="D87" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
+      <c r="F87" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="7"/>
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
@@ -2481,14 +2727,18 @@
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
+      <c r="D88" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-      <c r="K88" s="1"/>
+      <c r="F88" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7"/>
+      <c r="J88" s="7"/>
+      <c r="K88" s="7"/>
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
@@ -2508,14 +2758,14 @@
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
+      <c r="D89" s="2"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="1"/>
-      <c r="J89" s="1"/>
-      <c r="K89" s="1"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
+      <c r="I89" s="7"/>
+      <c r="J89" s="7"/>
+      <c r="K89" s="7"/>
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
@@ -2535,14 +2785,14 @@
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
+      <c r="D90" s="2"/>
       <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7"/>
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
@@ -2562,14 +2812,13 @@
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
+      <c r="D91" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-      <c r="K91" s="1"/>
+      <c r="F91" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
@@ -2591,12 +2840,6 @@
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
@@ -2618,12 +2861,6 @@
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-      <c r="K93" s="1"/>
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
@@ -2643,9 +2880,13 @@
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
+      <c r="D94" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
+      <c r="F94" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
@@ -3072,8 +3313,12 @@
       <c r="Y109" s="1"/>
     </row>
     <row r="110">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
+      <c r="A110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -3126,10 +3371,18 @@
       <c r="Y111" s="1"/>
     </row>
     <row r="112">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
+      <c r="A112" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B112" s="4">
+        <v>5000.0</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
@@ -26426,7 +26679,2825 @@
       <c r="X974" s="1"/>
       <c r="Y974" s="1"/>
     </row>
+    <row r="975">
+      <c r="A975" s="1"/>
+      <c r="B975" s="1"/>
+      <c r="C975" s="1"/>
+      <c r="D975" s="1"/>
+      <c r="E975" s="1"/>
+      <c r="F975" s="1"/>
+      <c r="G975" s="1"/>
+      <c r="H975" s="1"/>
+      <c r="I975" s="1"/>
+      <c r="J975" s="1"/>
+      <c r="K975" s="1"/>
+      <c r="L975" s="1"/>
+      <c r="M975" s="1"/>
+      <c r="N975" s="1"/>
+      <c r="O975" s="1"/>
+      <c r="P975" s="1"/>
+      <c r="Q975" s="1"/>
+      <c r="R975" s="1"/>
+      <c r="S975" s="1"/>
+      <c r="T975" s="1"/>
+      <c r="U975" s="1"/>
+      <c r="V975" s="1"/>
+      <c r="W975" s="1"/>
+      <c r="X975" s="1"/>
+      <c r="Y975" s="1"/>
+    </row>
+    <row r="976">
+      <c r="A976" s="1"/>
+      <c r="B976" s="1"/>
+      <c r="C976" s="1"/>
+      <c r="D976" s="1"/>
+      <c r="E976" s="1"/>
+      <c r="F976" s="1"/>
+      <c r="G976" s="1"/>
+      <c r="H976" s="1"/>
+      <c r="I976" s="1"/>
+      <c r="J976" s="1"/>
+      <c r="K976" s="1"/>
+      <c r="L976" s="1"/>
+      <c r="M976" s="1"/>
+      <c r="N976" s="1"/>
+      <c r="O976" s="1"/>
+      <c r="P976" s="1"/>
+      <c r="Q976" s="1"/>
+      <c r="R976" s="1"/>
+      <c r="S976" s="1"/>
+      <c r="T976" s="1"/>
+      <c r="U976" s="1"/>
+      <c r="V976" s="1"/>
+      <c r="W976" s="1"/>
+      <c r="X976" s="1"/>
+      <c r="Y976" s="1"/>
+    </row>
+    <row r="977">
+      <c r="A977" s="1"/>
+      <c r="B977" s="1"/>
+      <c r="C977" s="1"/>
+      <c r="D977" s="1"/>
+      <c r="E977" s="1"/>
+      <c r="F977" s="1"/>
+      <c r="G977" s="1"/>
+      <c r="H977" s="1"/>
+      <c r="I977" s="1"/>
+      <c r="J977" s="1"/>
+      <c r="K977" s="1"/>
+      <c r="L977" s="1"/>
+      <c r="M977" s="1"/>
+      <c r="N977" s="1"/>
+      <c r="O977" s="1"/>
+      <c r="P977" s="1"/>
+      <c r="Q977" s="1"/>
+      <c r="R977" s="1"/>
+      <c r="S977" s="1"/>
+      <c r="T977" s="1"/>
+      <c r="U977" s="1"/>
+      <c r="V977" s="1"/>
+      <c r="W977" s="1"/>
+      <c r="X977" s="1"/>
+      <c r="Y977" s="1"/>
+    </row>
+    <row r="978">
+      <c r="A978" s="1"/>
+      <c r="B978" s="1"/>
+      <c r="C978" s="1"/>
+      <c r="D978" s="1"/>
+      <c r="E978" s="1"/>
+      <c r="F978" s="1"/>
+      <c r="G978" s="1"/>
+      <c r="H978" s="1"/>
+      <c r="I978" s="1"/>
+      <c r="J978" s="1"/>
+      <c r="K978" s="1"/>
+      <c r="L978" s="1"/>
+      <c r="M978" s="1"/>
+      <c r="N978" s="1"/>
+      <c r="O978" s="1"/>
+      <c r="P978" s="1"/>
+      <c r="Q978" s="1"/>
+      <c r="R978" s="1"/>
+      <c r="S978" s="1"/>
+      <c r="T978" s="1"/>
+      <c r="U978" s="1"/>
+      <c r="V978" s="1"/>
+      <c r="W978" s="1"/>
+      <c r="X978" s="1"/>
+      <c r="Y978" s="1"/>
+    </row>
+    <row r="979">
+      <c r="A979" s="1"/>
+      <c r="B979" s="1"/>
+      <c r="C979" s="1"/>
+      <c r="D979" s="1"/>
+      <c r="E979" s="1"/>
+      <c r="F979" s="1"/>
+      <c r="G979" s="1"/>
+      <c r="H979" s="1"/>
+      <c r="I979" s="1"/>
+      <c r="J979" s="1"/>
+      <c r="K979" s="1"/>
+      <c r="L979" s="1"/>
+      <c r="M979" s="1"/>
+      <c r="N979" s="1"/>
+      <c r="O979" s="1"/>
+      <c r="P979" s="1"/>
+      <c r="Q979" s="1"/>
+      <c r="R979" s="1"/>
+      <c r="S979" s="1"/>
+      <c r="T979" s="1"/>
+      <c r="U979" s="1"/>
+      <c r="V979" s="1"/>
+      <c r="W979" s="1"/>
+      <c r="X979" s="1"/>
+      <c r="Y979" s="1"/>
+    </row>
+    <row r="980">
+      <c r="A980" s="1"/>
+      <c r="B980" s="1"/>
+      <c r="C980" s="1"/>
+      <c r="D980" s="1"/>
+      <c r="E980" s="1"/>
+      <c r="F980" s="1"/>
+      <c r="G980" s="1"/>
+      <c r="H980" s="1"/>
+      <c r="I980" s="1"/>
+      <c r="J980" s="1"/>
+      <c r="K980" s="1"/>
+      <c r="L980" s="1"/>
+      <c r="M980" s="1"/>
+      <c r="N980" s="1"/>
+      <c r="O980" s="1"/>
+      <c r="P980" s="1"/>
+      <c r="Q980" s="1"/>
+      <c r="R980" s="1"/>
+      <c r="S980" s="1"/>
+      <c r="T980" s="1"/>
+      <c r="U980" s="1"/>
+      <c r="V980" s="1"/>
+      <c r="W980" s="1"/>
+      <c r="X980" s="1"/>
+      <c r="Y980" s="1"/>
+    </row>
+    <row r="981">
+      <c r="A981" s="1"/>
+      <c r="B981" s="1"/>
+      <c r="C981" s="1"/>
+      <c r="D981" s="1"/>
+      <c r="E981" s="1"/>
+      <c r="F981" s="1"/>
+      <c r="G981" s="1"/>
+      <c r="H981" s="1"/>
+      <c r="I981" s="1"/>
+      <c r="J981" s="1"/>
+      <c r="K981" s="1"/>
+      <c r="L981" s="1"/>
+      <c r="M981" s="1"/>
+      <c r="N981" s="1"/>
+      <c r="O981" s="1"/>
+      <c r="P981" s="1"/>
+      <c r="Q981" s="1"/>
+      <c r="R981" s="1"/>
+      <c r="S981" s="1"/>
+      <c r="T981" s="1"/>
+      <c r="U981" s="1"/>
+      <c r="V981" s="1"/>
+      <c r="W981" s="1"/>
+      <c r="X981" s="1"/>
+      <c r="Y981" s="1"/>
+    </row>
+    <row r="982">
+      <c r="A982" s="1"/>
+      <c r="B982" s="1"/>
+      <c r="C982" s="1"/>
+      <c r="D982" s="1"/>
+      <c r="E982" s="1"/>
+      <c r="F982" s="1"/>
+      <c r="G982" s="1"/>
+      <c r="H982" s="1"/>
+      <c r="I982" s="1"/>
+      <c r="J982" s="1"/>
+      <c r="K982" s="1"/>
+      <c r="L982" s="1"/>
+      <c r="M982" s="1"/>
+      <c r="N982" s="1"/>
+      <c r="O982" s="1"/>
+      <c r="P982" s="1"/>
+      <c r="Q982" s="1"/>
+      <c r="R982" s="1"/>
+      <c r="S982" s="1"/>
+      <c r="T982" s="1"/>
+      <c r="U982" s="1"/>
+      <c r="V982" s="1"/>
+      <c r="W982" s="1"/>
+      <c r="X982" s="1"/>
+      <c r="Y982" s="1"/>
+    </row>
+    <row r="983">
+      <c r="A983" s="1"/>
+      <c r="B983" s="1"/>
+      <c r="C983" s="1"/>
+      <c r="D983" s="1"/>
+      <c r="E983" s="1"/>
+      <c r="F983" s="1"/>
+      <c r="G983" s="1"/>
+      <c r="H983" s="1"/>
+      <c r="I983" s="1"/>
+      <c r="J983" s="1"/>
+      <c r="K983" s="1"/>
+      <c r="L983" s="1"/>
+      <c r="M983" s="1"/>
+      <c r="N983" s="1"/>
+      <c r="O983" s="1"/>
+      <c r="P983" s="1"/>
+      <c r="Q983" s="1"/>
+      <c r="R983" s="1"/>
+      <c r="S983" s="1"/>
+      <c r="T983" s="1"/>
+      <c r="U983" s="1"/>
+      <c r="V983" s="1"/>
+      <c r="W983" s="1"/>
+      <c r="X983" s="1"/>
+      <c r="Y983" s="1"/>
+    </row>
+    <row r="984">
+      <c r="A984" s="1"/>
+      <c r="B984" s="1"/>
+      <c r="C984" s="1"/>
+      <c r="D984" s="1"/>
+      <c r="E984" s="1"/>
+      <c r="F984" s="1"/>
+      <c r="G984" s="1"/>
+      <c r="H984" s="1"/>
+      <c r="I984" s="1"/>
+      <c r="J984" s="1"/>
+      <c r="K984" s="1"/>
+      <c r="L984" s="1"/>
+      <c r="M984" s="1"/>
+      <c r="N984" s="1"/>
+      <c r="O984" s="1"/>
+      <c r="P984" s="1"/>
+      <c r="Q984" s="1"/>
+      <c r="R984" s="1"/>
+      <c r="S984" s="1"/>
+      <c r="T984" s="1"/>
+      <c r="U984" s="1"/>
+      <c r="V984" s="1"/>
+      <c r="W984" s="1"/>
+      <c r="X984" s="1"/>
+      <c r="Y984" s="1"/>
+    </row>
+    <row r="985">
+      <c r="A985" s="1"/>
+      <c r="B985" s="1"/>
+      <c r="C985" s="1"/>
+      <c r="D985" s="1"/>
+      <c r="E985" s="1"/>
+      <c r="F985" s="1"/>
+      <c r="G985" s="1"/>
+      <c r="H985" s="1"/>
+      <c r="I985" s="1"/>
+      <c r="J985" s="1"/>
+      <c r="K985" s="1"/>
+      <c r="L985" s="1"/>
+      <c r="M985" s="1"/>
+      <c r="N985" s="1"/>
+      <c r="O985" s="1"/>
+      <c r="P985" s="1"/>
+      <c r="Q985" s="1"/>
+      <c r="R985" s="1"/>
+      <c r="S985" s="1"/>
+      <c r="T985" s="1"/>
+      <c r="U985" s="1"/>
+      <c r="V985" s="1"/>
+      <c r="W985" s="1"/>
+      <c r="X985" s="1"/>
+      <c r="Y985" s="1"/>
+    </row>
+    <row r="986">
+      <c r="A986" s="1"/>
+      <c r="B986" s="1"/>
+      <c r="C986" s="1"/>
+      <c r="D986" s="1"/>
+      <c r="E986" s="1"/>
+      <c r="F986" s="1"/>
+      <c r="G986" s="1"/>
+      <c r="H986" s="1"/>
+      <c r="I986" s="1"/>
+      <c r="J986" s="1"/>
+      <c r="K986" s="1"/>
+      <c r="L986" s="1"/>
+      <c r="M986" s="1"/>
+      <c r="N986" s="1"/>
+      <c r="O986" s="1"/>
+      <c r="P986" s="1"/>
+      <c r="Q986" s="1"/>
+      <c r="R986" s="1"/>
+      <c r="S986" s="1"/>
+      <c r="T986" s="1"/>
+      <c r="U986" s="1"/>
+      <c r="V986" s="1"/>
+      <c r="W986" s="1"/>
+      <c r="X986" s="1"/>
+      <c r="Y986" s="1"/>
+    </row>
+    <row r="987">
+      <c r="A987" s="1"/>
+      <c r="B987" s="1"/>
+      <c r="C987" s="1"/>
+      <c r="D987" s="1"/>
+      <c r="E987" s="1"/>
+      <c r="F987" s="1"/>
+      <c r="G987" s="1"/>
+      <c r="H987" s="1"/>
+      <c r="I987" s="1"/>
+      <c r="J987" s="1"/>
+      <c r="K987" s="1"/>
+      <c r="L987" s="1"/>
+      <c r="M987" s="1"/>
+      <c r="N987" s="1"/>
+      <c r="O987" s="1"/>
+      <c r="P987" s="1"/>
+      <c r="Q987" s="1"/>
+      <c r="R987" s="1"/>
+      <c r="S987" s="1"/>
+      <c r="T987" s="1"/>
+      <c r="U987" s="1"/>
+      <c r="V987" s="1"/>
+      <c r="W987" s="1"/>
+      <c r="X987" s="1"/>
+      <c r="Y987" s="1"/>
+    </row>
+    <row r="988">
+      <c r="A988" s="1"/>
+      <c r="B988" s="1"/>
+      <c r="C988" s="1"/>
+      <c r="D988" s="1"/>
+      <c r="E988" s="1"/>
+      <c r="F988" s="1"/>
+      <c r="G988" s="1"/>
+      <c r="H988" s="1"/>
+      <c r="I988" s="1"/>
+      <c r="J988" s="1"/>
+      <c r="K988" s="1"/>
+      <c r="L988" s="1"/>
+      <c r="M988" s="1"/>
+      <c r="N988" s="1"/>
+      <c r="O988" s="1"/>
+      <c r="P988" s="1"/>
+      <c r="Q988" s="1"/>
+      <c r="R988" s="1"/>
+      <c r="S988" s="1"/>
+      <c r="T988" s="1"/>
+      <c r="U988" s="1"/>
+      <c r="V988" s="1"/>
+      <c r="W988" s="1"/>
+      <c r="X988" s="1"/>
+      <c r="Y988" s="1"/>
+    </row>
+    <row r="989">
+      <c r="A989" s="1"/>
+      <c r="B989" s="1"/>
+      <c r="C989" s="1"/>
+      <c r="D989" s="1"/>
+      <c r="E989" s="1"/>
+      <c r="F989" s="1"/>
+      <c r="G989" s="1"/>
+      <c r="H989" s="1"/>
+      <c r="I989" s="1"/>
+      <c r="J989" s="1"/>
+      <c r="K989" s="1"/>
+      <c r="L989" s="1"/>
+      <c r="M989" s="1"/>
+      <c r="N989" s="1"/>
+      <c r="O989" s="1"/>
+      <c r="P989" s="1"/>
+      <c r="Q989" s="1"/>
+      <c r="R989" s="1"/>
+      <c r="S989" s="1"/>
+      <c r="T989" s="1"/>
+      <c r="U989" s="1"/>
+      <c r="V989" s="1"/>
+      <c r="W989" s="1"/>
+      <c r="X989" s="1"/>
+      <c r="Y989" s="1"/>
+    </row>
+    <row r="990">
+      <c r="A990" s="1"/>
+      <c r="B990" s="1"/>
+      <c r="C990" s="1"/>
+      <c r="D990" s="1"/>
+      <c r="E990" s="1"/>
+      <c r="F990" s="1"/>
+      <c r="G990" s="1"/>
+      <c r="H990" s="1"/>
+      <c r="I990" s="1"/>
+      <c r="J990" s="1"/>
+      <c r="K990" s="1"/>
+      <c r="L990" s="1"/>
+      <c r="M990" s="1"/>
+      <c r="N990" s="1"/>
+      <c r="O990" s="1"/>
+      <c r="P990" s="1"/>
+      <c r="Q990" s="1"/>
+      <c r="R990" s="1"/>
+      <c r="S990" s="1"/>
+      <c r="T990" s="1"/>
+      <c r="U990" s="1"/>
+      <c r="V990" s="1"/>
+      <c r="W990" s="1"/>
+      <c r="X990" s="1"/>
+      <c r="Y990" s="1"/>
+    </row>
+    <row r="991">
+      <c r="A991" s="1"/>
+      <c r="B991" s="1"/>
+      <c r="C991" s="1"/>
+      <c r="D991" s="1"/>
+      <c r="E991" s="1"/>
+      <c r="F991" s="1"/>
+      <c r="G991" s="1"/>
+      <c r="H991" s="1"/>
+      <c r="I991" s="1"/>
+      <c r="J991" s="1"/>
+      <c r="K991" s="1"/>
+      <c r="L991" s="1"/>
+      <c r="M991" s="1"/>
+      <c r="N991" s="1"/>
+      <c r="O991" s="1"/>
+      <c r="P991" s="1"/>
+      <c r="Q991" s="1"/>
+      <c r="R991" s="1"/>
+      <c r="S991" s="1"/>
+      <c r="T991" s="1"/>
+      <c r="U991" s="1"/>
+      <c r="V991" s="1"/>
+      <c r="W991" s="1"/>
+      <c r="X991" s="1"/>
+      <c r="Y991" s="1"/>
+    </row>
+    <row r="992">
+      <c r="A992" s="1"/>
+      <c r="B992" s="1"/>
+      <c r="C992" s="1"/>
+      <c r="D992" s="1"/>
+      <c r="E992" s="1"/>
+      <c r="F992" s="1"/>
+      <c r="G992" s="1"/>
+      <c r="H992" s="1"/>
+      <c r="I992" s="1"/>
+      <c r="J992" s="1"/>
+      <c r="K992" s="1"/>
+      <c r="L992" s="1"/>
+      <c r="M992" s="1"/>
+      <c r="N992" s="1"/>
+      <c r="O992" s="1"/>
+      <c r="P992" s="1"/>
+      <c r="Q992" s="1"/>
+      <c r="R992" s="1"/>
+      <c r="S992" s="1"/>
+      <c r="T992" s="1"/>
+      <c r="U992" s="1"/>
+      <c r="V992" s="1"/>
+      <c r="W992" s="1"/>
+      <c r="X992" s="1"/>
+      <c r="Y992" s="1"/>
+    </row>
+    <row r="993">
+      <c r="A993" s="1"/>
+      <c r="B993" s="1"/>
+      <c r="C993" s="1"/>
+      <c r="D993" s="1"/>
+      <c r="E993" s="1"/>
+      <c r="F993" s="1"/>
+      <c r="G993" s="1"/>
+      <c r="H993" s="1"/>
+      <c r="I993" s="1"/>
+      <c r="J993" s="1"/>
+      <c r="K993" s="1"/>
+      <c r="L993" s="1"/>
+      <c r="M993" s="1"/>
+      <c r="N993" s="1"/>
+      <c r="O993" s="1"/>
+      <c r="P993" s="1"/>
+      <c r="Q993" s="1"/>
+      <c r="R993" s="1"/>
+      <c r="S993" s="1"/>
+      <c r="T993" s="1"/>
+      <c r="U993" s="1"/>
+      <c r="V993" s="1"/>
+      <c r="W993" s="1"/>
+      <c r="X993" s="1"/>
+      <c r="Y993" s="1"/>
+    </row>
+    <row r="994">
+      <c r="A994" s="1"/>
+      <c r="B994" s="1"/>
+      <c r="C994" s="1"/>
+      <c r="D994" s="1"/>
+      <c r="E994" s="1"/>
+      <c r="F994" s="1"/>
+      <c r="G994" s="1"/>
+      <c r="H994" s="1"/>
+      <c r="I994" s="1"/>
+      <c r="J994" s="1"/>
+      <c r="K994" s="1"/>
+      <c r="L994" s="1"/>
+      <c r="M994" s="1"/>
+      <c r="N994" s="1"/>
+      <c r="O994" s="1"/>
+      <c r="P994" s="1"/>
+      <c r="Q994" s="1"/>
+      <c r="R994" s="1"/>
+      <c r="S994" s="1"/>
+      <c r="T994" s="1"/>
+      <c r="U994" s="1"/>
+      <c r="V994" s="1"/>
+      <c r="W994" s="1"/>
+      <c r="X994" s="1"/>
+      <c r="Y994" s="1"/>
+    </row>
+    <row r="995">
+      <c r="A995" s="1"/>
+      <c r="B995" s="1"/>
+      <c r="C995" s="1"/>
+      <c r="D995" s="1"/>
+      <c r="E995" s="1"/>
+      <c r="F995" s="1"/>
+      <c r="G995" s="1"/>
+      <c r="H995" s="1"/>
+      <c r="I995" s="1"/>
+      <c r="J995" s="1"/>
+      <c r="K995" s="1"/>
+      <c r="L995" s="1"/>
+      <c r="M995" s="1"/>
+      <c r="N995" s="1"/>
+      <c r="O995" s="1"/>
+      <c r="P995" s="1"/>
+      <c r="Q995" s="1"/>
+      <c r="R995" s="1"/>
+      <c r="S995" s="1"/>
+      <c r="T995" s="1"/>
+      <c r="U995" s="1"/>
+      <c r="V995" s="1"/>
+      <c r="W995" s="1"/>
+      <c r="X995" s="1"/>
+      <c r="Y995" s="1"/>
+    </row>
+    <row r="996">
+      <c r="A996" s="1"/>
+      <c r="B996" s="1"/>
+      <c r="C996" s="1"/>
+      <c r="D996" s="1"/>
+      <c r="E996" s="1"/>
+      <c r="F996" s="1"/>
+      <c r="G996" s="1"/>
+      <c r="H996" s="1"/>
+      <c r="I996" s="1"/>
+      <c r="J996" s="1"/>
+      <c r="K996" s="1"/>
+      <c r="L996" s="1"/>
+      <c r="M996" s="1"/>
+      <c r="N996" s="1"/>
+      <c r="O996" s="1"/>
+      <c r="P996" s="1"/>
+      <c r="Q996" s="1"/>
+      <c r="R996" s="1"/>
+      <c r="S996" s="1"/>
+      <c r="T996" s="1"/>
+      <c r="U996" s="1"/>
+      <c r="V996" s="1"/>
+      <c r="W996" s="1"/>
+      <c r="X996" s="1"/>
+      <c r="Y996" s="1"/>
+    </row>
+    <row r="997">
+      <c r="A997" s="1"/>
+      <c r="B997" s="1"/>
+      <c r="C997" s="1"/>
+      <c r="D997" s="1"/>
+      <c r="E997" s="1"/>
+      <c r="F997" s="1"/>
+      <c r="G997" s="1"/>
+      <c r="H997" s="1"/>
+      <c r="I997" s="1"/>
+      <c r="J997" s="1"/>
+      <c r="K997" s="1"/>
+      <c r="L997" s="1"/>
+      <c r="M997" s="1"/>
+      <c r="N997" s="1"/>
+      <c r="O997" s="1"/>
+      <c r="P997" s="1"/>
+      <c r="Q997" s="1"/>
+      <c r="R997" s="1"/>
+      <c r="S997" s="1"/>
+      <c r="T997" s="1"/>
+      <c r="U997" s="1"/>
+      <c r="V997" s="1"/>
+      <c r="W997" s="1"/>
+      <c r="X997" s="1"/>
+      <c r="Y997" s="1"/>
+    </row>
+    <row r="998">
+      <c r="A998" s="1"/>
+      <c r="B998" s="1"/>
+      <c r="C998" s="1"/>
+      <c r="D998" s="1"/>
+      <c r="E998" s="1"/>
+      <c r="F998" s="1"/>
+      <c r="G998" s="1"/>
+      <c r="H998" s="1"/>
+      <c r="I998" s="1"/>
+      <c r="J998" s="1"/>
+      <c r="K998" s="1"/>
+      <c r="L998" s="1"/>
+      <c r="M998" s="1"/>
+      <c r="N998" s="1"/>
+      <c r="O998" s="1"/>
+      <c r="P998" s="1"/>
+      <c r="Q998" s="1"/>
+      <c r="R998" s="1"/>
+      <c r="S998" s="1"/>
+      <c r="T998" s="1"/>
+      <c r="U998" s="1"/>
+      <c r="V998" s="1"/>
+      <c r="W998" s="1"/>
+      <c r="X998" s="1"/>
+      <c r="Y998" s="1"/>
+    </row>
+    <row r="999">
+      <c r="A999" s="1"/>
+      <c r="B999" s="1"/>
+      <c r="C999" s="1"/>
+      <c r="D999" s="1"/>
+      <c r="E999" s="1"/>
+      <c r="F999" s="1"/>
+      <c r="G999" s="1"/>
+      <c r="H999" s="1"/>
+      <c r="I999" s="1"/>
+      <c r="J999" s="1"/>
+      <c r="K999" s="1"/>
+      <c r="L999" s="1"/>
+      <c r="M999" s="1"/>
+      <c r="N999" s="1"/>
+      <c r="O999" s="1"/>
+      <c r="P999" s="1"/>
+      <c r="Q999" s="1"/>
+      <c r="R999" s="1"/>
+      <c r="S999" s="1"/>
+      <c r="T999" s="1"/>
+      <c r="U999" s="1"/>
+      <c r="V999" s="1"/>
+      <c r="W999" s="1"/>
+      <c r="X999" s="1"/>
+      <c r="Y999" s="1"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="1"/>
+      <c r="B1000" s="1"/>
+      <c r="C1000" s="1"/>
+      <c r="D1000" s="1"/>
+      <c r="E1000" s="1"/>
+      <c r="F1000" s="1"/>
+      <c r="G1000" s="1"/>
+      <c r="H1000" s="1"/>
+      <c r="I1000" s="1"/>
+      <c r="J1000" s="1"/>
+      <c r="K1000" s="1"/>
+      <c r="L1000" s="1"/>
+      <c r="M1000" s="1"/>
+      <c r="N1000" s="1"/>
+      <c r="O1000" s="1"/>
+      <c r="P1000" s="1"/>
+      <c r="Q1000" s="1"/>
+      <c r="R1000" s="1"/>
+      <c r="S1000" s="1"/>
+      <c r="T1000" s="1"/>
+      <c r="U1000" s="1"/>
+      <c r="V1000" s="1"/>
+      <c r="W1000" s="1"/>
+      <c r="X1000" s="1"/>
+      <c r="Y1000" s="1"/>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="1"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="1"/>
+      <c r="G1001" s="1"/>
+      <c r="H1001" s="1"/>
+      <c r="I1001" s="1"/>
+      <c r="J1001" s="1"/>
+      <c r="K1001" s="1"/>
+      <c r="L1001" s="1"/>
+      <c r="M1001" s="1"/>
+      <c r="N1001" s="1"/>
+      <c r="O1001" s="1"/>
+      <c r="P1001" s="1"/>
+      <c r="Q1001" s="1"/>
+      <c r="R1001" s="1"/>
+      <c r="S1001" s="1"/>
+      <c r="T1001" s="1"/>
+      <c r="U1001" s="1"/>
+      <c r="V1001" s="1"/>
+      <c r="W1001" s="1"/>
+      <c r="X1001" s="1"/>
+      <c r="Y1001" s="1"/>
+    </row>
+    <row r="1002">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="1"/>
+      <c r="G1002" s="1"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="1"/>
+      <c r="J1002" s="1"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+      <c r="Q1002" s="1"/>
+      <c r="R1002" s="1"/>
+      <c r="S1002" s="1"/>
+      <c r="T1002" s="1"/>
+      <c r="U1002" s="1"/>
+      <c r="V1002" s="1"/>
+      <c r="W1002" s="1"/>
+      <c r="X1002" s="1"/>
+      <c r="Y1002" s="1"/>
+    </row>
+    <row r="1003">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="1"/>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1"/>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="1"/>
+      <c r="K1004" s="1"/>
+      <c r="L1004" s="1"/>
+      <c r="M1004" s="1"/>
+      <c r="N1004" s="1"/>
+      <c r="O1004" s="1"/>
+      <c r="P1004" s="1"/>
+      <c r="Q1004" s="1"/>
+      <c r="R1004" s="1"/>
+      <c r="S1004" s="1"/>
+      <c r="T1004" s="1"/>
+      <c r="U1004" s="1"/>
+      <c r="V1004" s="1"/>
+      <c r="W1004" s="1"/>
+      <c r="X1004" s="1"/>
+      <c r="Y1004" s="1"/>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="1"/>
+      <c r="E1005" s="1"/>
+      <c r="F1005" s="1"/>
+      <c r="G1005" s="1"/>
+      <c r="H1005" s="1"/>
+      <c r="I1005" s="1"/>
+      <c r="J1005" s="1"/>
+      <c r="K1005" s="1"/>
+      <c r="L1005" s="1"/>
+      <c r="M1005" s="1"/>
+      <c r="N1005" s="1"/>
+      <c r="O1005" s="1"/>
+      <c r="P1005" s="1"/>
+      <c r="Q1005" s="1"/>
+      <c r="R1005" s="1"/>
+      <c r="S1005" s="1"/>
+      <c r="T1005" s="1"/>
+      <c r="U1005" s="1"/>
+      <c r="V1005" s="1"/>
+      <c r="W1005" s="1"/>
+      <c r="X1005" s="1"/>
+      <c r="Y1005" s="1"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="1"/>
+      <c r="E1006" s="1"/>
+      <c r="F1006" s="1"/>
+      <c r="G1006" s="1"/>
+      <c r="H1006" s="1"/>
+      <c r="I1006" s="1"/>
+      <c r="J1006" s="1"/>
+      <c r="K1006" s="1"/>
+      <c r="L1006" s="1"/>
+      <c r="M1006" s="1"/>
+      <c r="N1006" s="1"/>
+      <c r="O1006" s="1"/>
+      <c r="P1006" s="1"/>
+      <c r="Q1006" s="1"/>
+      <c r="R1006" s="1"/>
+      <c r="S1006" s="1"/>
+      <c r="T1006" s="1"/>
+      <c r="U1006" s="1"/>
+      <c r="V1006" s="1"/>
+      <c r="W1006" s="1"/>
+      <c r="X1006" s="1"/>
+      <c r="Y1006" s="1"/>
+    </row>
+    <row r="1007">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="1"/>
+      <c r="E1007" s="1"/>
+      <c r="F1007" s="1"/>
+      <c r="G1007" s="1"/>
+      <c r="H1007" s="1"/>
+      <c r="I1007" s="1"/>
+      <c r="J1007" s="1"/>
+      <c r="K1007" s="1"/>
+      <c r="L1007" s="1"/>
+      <c r="M1007" s="1"/>
+      <c r="N1007" s="1"/>
+      <c r="O1007" s="1"/>
+      <c r="P1007" s="1"/>
+      <c r="Q1007" s="1"/>
+      <c r="R1007" s="1"/>
+      <c r="S1007" s="1"/>
+      <c r="T1007" s="1"/>
+      <c r="U1007" s="1"/>
+      <c r="V1007" s="1"/>
+      <c r="W1007" s="1"/>
+      <c r="X1007" s="1"/>
+      <c r="Y1007" s="1"/>
+    </row>
+    <row r="1008">
+      <c r="A1008" s="1"/>
+      <c r="B1008" s="1"/>
+      <c r="C1008" s="1"/>
+      <c r="D1008" s="1"/>
+      <c r="E1008" s="1"/>
+      <c r="F1008" s="1"/>
+      <c r="G1008" s="1"/>
+      <c r="H1008" s="1"/>
+      <c r="I1008" s="1"/>
+      <c r="J1008" s="1"/>
+      <c r="K1008" s="1"/>
+      <c r="L1008" s="1"/>
+      <c r="M1008" s="1"/>
+      <c r="N1008" s="1"/>
+      <c r="O1008" s="1"/>
+      <c r="P1008" s="1"/>
+      <c r="Q1008" s="1"/>
+      <c r="R1008" s="1"/>
+      <c r="S1008" s="1"/>
+      <c r="T1008" s="1"/>
+      <c r="U1008" s="1"/>
+      <c r="V1008" s="1"/>
+      <c r="W1008" s="1"/>
+      <c r="X1008" s="1"/>
+      <c r="Y1008" s="1"/>
+    </row>
+    <row r="1009">
+      <c r="A1009" s="1"/>
+      <c r="B1009" s="1"/>
+      <c r="C1009" s="1"/>
+      <c r="D1009" s="1"/>
+      <c r="E1009" s="1"/>
+      <c r="F1009" s="1"/>
+      <c r="G1009" s="1"/>
+      <c r="H1009" s="1"/>
+      <c r="I1009" s="1"/>
+      <c r="J1009" s="1"/>
+      <c r="K1009" s="1"/>
+      <c r="L1009" s="1"/>
+      <c r="M1009" s="1"/>
+      <c r="N1009" s="1"/>
+      <c r="O1009" s="1"/>
+      <c r="P1009" s="1"/>
+      <c r="Q1009" s="1"/>
+      <c r="R1009" s="1"/>
+      <c r="S1009" s="1"/>
+      <c r="T1009" s="1"/>
+      <c r="U1009" s="1"/>
+      <c r="V1009" s="1"/>
+      <c r="W1009" s="1"/>
+      <c r="X1009" s="1"/>
+      <c r="Y1009" s="1"/>
+    </row>
+    <row r="1010">
+      <c r="A1010" s="1"/>
+      <c r="B1010" s="1"/>
+      <c r="C1010" s="1"/>
+      <c r="D1010" s="1"/>
+      <c r="E1010" s="1"/>
+      <c r="F1010" s="1"/>
+      <c r="G1010" s="1"/>
+      <c r="H1010" s="1"/>
+      <c r="I1010" s="1"/>
+      <c r="J1010" s="1"/>
+      <c r="K1010" s="1"/>
+      <c r="L1010" s="1"/>
+      <c r="M1010" s="1"/>
+      <c r="N1010" s="1"/>
+      <c r="O1010" s="1"/>
+      <c r="P1010" s="1"/>
+      <c r="Q1010" s="1"/>
+      <c r="R1010" s="1"/>
+      <c r="S1010" s="1"/>
+      <c r="T1010" s="1"/>
+      <c r="U1010" s="1"/>
+      <c r="V1010" s="1"/>
+      <c r="W1010" s="1"/>
+      <c r="X1010" s="1"/>
+      <c r="Y1010" s="1"/>
+    </row>
+    <row r="1011">
+      <c r="A1011" s="1"/>
+      <c r="B1011" s="1"/>
+      <c r="C1011" s="1"/>
+      <c r="D1011" s="1"/>
+      <c r="E1011" s="1"/>
+      <c r="F1011" s="1"/>
+      <c r="G1011" s="1"/>
+      <c r="H1011" s="1"/>
+      <c r="I1011" s="1"/>
+      <c r="J1011" s="1"/>
+      <c r="K1011" s="1"/>
+      <c r="L1011" s="1"/>
+      <c r="M1011" s="1"/>
+      <c r="N1011" s="1"/>
+      <c r="O1011" s="1"/>
+      <c r="P1011" s="1"/>
+      <c r="Q1011" s="1"/>
+      <c r="R1011" s="1"/>
+      <c r="S1011" s="1"/>
+      <c r="T1011" s="1"/>
+      <c r="U1011" s="1"/>
+      <c r="V1011" s="1"/>
+      <c r="W1011" s="1"/>
+      <c r="X1011" s="1"/>
+      <c r="Y1011" s="1"/>
+    </row>
+    <row r="1012">
+      <c r="A1012" s="1"/>
+      <c r="B1012" s="1"/>
+      <c r="C1012" s="1"/>
+      <c r="D1012" s="1"/>
+      <c r="E1012" s="1"/>
+      <c r="F1012" s="1"/>
+      <c r="G1012" s="1"/>
+      <c r="H1012" s="1"/>
+      <c r="I1012" s="1"/>
+      <c r="J1012" s="1"/>
+      <c r="K1012" s="1"/>
+      <c r="L1012" s="1"/>
+      <c r="M1012" s="1"/>
+      <c r="N1012" s="1"/>
+      <c r="O1012" s="1"/>
+      <c r="P1012" s="1"/>
+      <c r="Q1012" s="1"/>
+      <c r="R1012" s="1"/>
+      <c r="S1012" s="1"/>
+      <c r="T1012" s="1"/>
+      <c r="U1012" s="1"/>
+      <c r="V1012" s="1"/>
+      <c r="W1012" s="1"/>
+      <c r="X1012" s="1"/>
+      <c r="Y1012" s="1"/>
+    </row>
+    <row r="1013">
+      <c r="A1013" s="1"/>
+      <c r="B1013" s="1"/>
+      <c r="C1013" s="1"/>
+      <c r="D1013" s="1"/>
+      <c r="E1013" s="1"/>
+      <c r="F1013" s="1"/>
+      <c r="G1013" s="1"/>
+      <c r="H1013" s="1"/>
+      <c r="I1013" s="1"/>
+      <c r="J1013" s="1"/>
+      <c r="K1013" s="1"/>
+      <c r="L1013" s="1"/>
+      <c r="M1013" s="1"/>
+      <c r="N1013" s="1"/>
+      <c r="O1013" s="1"/>
+      <c r="P1013" s="1"/>
+      <c r="Q1013" s="1"/>
+      <c r="R1013" s="1"/>
+      <c r="S1013" s="1"/>
+      <c r="T1013" s="1"/>
+      <c r="U1013" s="1"/>
+      <c r="V1013" s="1"/>
+      <c r="W1013" s="1"/>
+      <c r="X1013" s="1"/>
+      <c r="Y1013" s="1"/>
+    </row>
+    <row r="1014">
+      <c r="A1014" s="1"/>
+      <c r="B1014" s="1"/>
+      <c r="C1014" s="1"/>
+      <c r="D1014" s="1"/>
+      <c r="E1014" s="1"/>
+      <c r="F1014" s="1"/>
+      <c r="G1014" s="1"/>
+      <c r="H1014" s="1"/>
+      <c r="I1014" s="1"/>
+      <c r="J1014" s="1"/>
+      <c r="K1014" s="1"/>
+      <c r="L1014" s="1"/>
+      <c r="M1014" s="1"/>
+      <c r="N1014" s="1"/>
+      <c r="O1014" s="1"/>
+      <c r="P1014" s="1"/>
+      <c r="Q1014" s="1"/>
+      <c r="R1014" s="1"/>
+      <c r="S1014" s="1"/>
+      <c r="T1014" s="1"/>
+      <c r="U1014" s="1"/>
+      <c r="V1014" s="1"/>
+      <c r="W1014" s="1"/>
+      <c r="X1014" s="1"/>
+      <c r="Y1014" s="1"/>
+    </row>
+    <row r="1015">
+      <c r="A1015" s="1"/>
+      <c r="B1015" s="1"/>
+      <c r="C1015" s="1"/>
+      <c r="D1015" s="1"/>
+      <c r="E1015" s="1"/>
+      <c r="F1015" s="1"/>
+      <c r="G1015" s="1"/>
+      <c r="H1015" s="1"/>
+      <c r="I1015" s="1"/>
+      <c r="J1015" s="1"/>
+      <c r="K1015" s="1"/>
+      <c r="L1015" s="1"/>
+      <c r="M1015" s="1"/>
+      <c r="N1015" s="1"/>
+      <c r="O1015" s="1"/>
+      <c r="P1015" s="1"/>
+      <c r="Q1015" s="1"/>
+      <c r="R1015" s="1"/>
+      <c r="S1015" s="1"/>
+      <c r="T1015" s="1"/>
+      <c r="U1015" s="1"/>
+      <c r="V1015" s="1"/>
+      <c r="W1015" s="1"/>
+      <c r="X1015" s="1"/>
+      <c r="Y1015" s="1"/>
+    </row>
+    <row r="1016">
+      <c r="A1016" s="1"/>
+      <c r="B1016" s="1"/>
+      <c r="C1016" s="1"/>
+      <c r="D1016" s="1"/>
+      <c r="E1016" s="1"/>
+      <c r="F1016" s="1"/>
+      <c r="G1016" s="1"/>
+      <c r="H1016" s="1"/>
+      <c r="I1016" s="1"/>
+      <c r="J1016" s="1"/>
+      <c r="K1016" s="1"/>
+      <c r="L1016" s="1"/>
+      <c r="M1016" s="1"/>
+      <c r="N1016" s="1"/>
+      <c r="O1016" s="1"/>
+      <c r="P1016" s="1"/>
+      <c r="Q1016" s="1"/>
+      <c r="R1016" s="1"/>
+      <c r="S1016" s="1"/>
+      <c r="T1016" s="1"/>
+      <c r="U1016" s="1"/>
+      <c r="V1016" s="1"/>
+      <c r="W1016" s="1"/>
+      <c r="X1016" s="1"/>
+      <c r="Y1016" s="1"/>
+    </row>
+    <row r="1017">
+      <c r="A1017" s="1"/>
+      <c r="B1017" s="1"/>
+      <c r="C1017" s="1"/>
+      <c r="D1017" s="1"/>
+      <c r="E1017" s="1"/>
+      <c r="F1017" s="1"/>
+      <c r="G1017" s="1"/>
+      <c r="H1017" s="1"/>
+      <c r="I1017" s="1"/>
+      <c r="J1017" s="1"/>
+      <c r="K1017" s="1"/>
+      <c r="L1017" s="1"/>
+      <c r="M1017" s="1"/>
+      <c r="N1017" s="1"/>
+      <c r="O1017" s="1"/>
+      <c r="P1017" s="1"/>
+      <c r="Q1017" s="1"/>
+      <c r="R1017" s="1"/>
+      <c r="S1017" s="1"/>
+      <c r="T1017" s="1"/>
+      <c r="U1017" s="1"/>
+      <c r="V1017" s="1"/>
+      <c r="W1017" s="1"/>
+      <c r="X1017" s="1"/>
+      <c r="Y1017" s="1"/>
+    </row>
+    <row r="1018">
+      <c r="A1018" s="1"/>
+      <c r="B1018" s="1"/>
+      <c r="C1018" s="1"/>
+      <c r="D1018" s="1"/>
+      <c r="E1018" s="1"/>
+      <c r="F1018" s="1"/>
+      <c r="G1018" s="1"/>
+      <c r="H1018" s="1"/>
+      <c r="I1018" s="1"/>
+      <c r="J1018" s="1"/>
+      <c r="K1018" s="1"/>
+      <c r="L1018" s="1"/>
+      <c r="M1018" s="1"/>
+      <c r="N1018" s="1"/>
+      <c r="O1018" s="1"/>
+      <c r="P1018" s="1"/>
+      <c r="Q1018" s="1"/>
+      <c r="R1018" s="1"/>
+      <c r="S1018" s="1"/>
+      <c r="T1018" s="1"/>
+      <c r="U1018" s="1"/>
+      <c r="V1018" s="1"/>
+      <c r="W1018" s="1"/>
+      <c r="X1018" s="1"/>
+      <c r="Y1018" s="1"/>
+    </row>
+    <row r="1019">
+      <c r="A1019" s="1"/>
+      <c r="B1019" s="1"/>
+      <c r="C1019" s="1"/>
+      <c r="D1019" s="1"/>
+      <c r="E1019" s="1"/>
+      <c r="F1019" s="1"/>
+      <c r="G1019" s="1"/>
+      <c r="H1019" s="1"/>
+      <c r="I1019" s="1"/>
+      <c r="J1019" s="1"/>
+      <c r="K1019" s="1"/>
+      <c r="L1019" s="1"/>
+      <c r="M1019" s="1"/>
+      <c r="N1019" s="1"/>
+      <c r="O1019" s="1"/>
+      <c r="P1019" s="1"/>
+      <c r="Q1019" s="1"/>
+      <c r="R1019" s="1"/>
+      <c r="S1019" s="1"/>
+      <c r="T1019" s="1"/>
+      <c r="U1019" s="1"/>
+      <c r="V1019" s="1"/>
+      <c r="W1019" s="1"/>
+      <c r="X1019" s="1"/>
+      <c r="Y1019" s="1"/>
+    </row>
+    <row r="1020">
+      <c r="A1020" s="1"/>
+      <c r="B1020" s="1"/>
+      <c r="C1020" s="1"/>
+      <c r="D1020" s="1"/>
+      <c r="E1020" s="1"/>
+      <c r="F1020" s="1"/>
+      <c r="G1020" s="1"/>
+      <c r="H1020" s="1"/>
+      <c r="I1020" s="1"/>
+      <c r="J1020" s="1"/>
+      <c r="K1020" s="1"/>
+      <c r="L1020" s="1"/>
+      <c r="M1020" s="1"/>
+      <c r="N1020" s="1"/>
+      <c r="O1020" s="1"/>
+      <c r="P1020" s="1"/>
+      <c r="Q1020" s="1"/>
+      <c r="R1020" s="1"/>
+      <c r="S1020" s="1"/>
+      <c r="T1020" s="1"/>
+      <c r="U1020" s="1"/>
+      <c r="V1020" s="1"/>
+      <c r="W1020" s="1"/>
+      <c r="X1020" s="1"/>
+      <c r="Y1020" s="1"/>
+    </row>
+    <row r="1021">
+      <c r="A1021" s="1"/>
+      <c r="B1021" s="1"/>
+      <c r="C1021" s="1"/>
+      <c r="D1021" s="1"/>
+      <c r="E1021" s="1"/>
+      <c r="F1021" s="1"/>
+      <c r="G1021" s="1"/>
+      <c r="H1021" s="1"/>
+      <c r="I1021" s="1"/>
+      <c r="J1021" s="1"/>
+      <c r="K1021" s="1"/>
+      <c r="L1021" s="1"/>
+      <c r="M1021" s="1"/>
+      <c r="N1021" s="1"/>
+      <c r="O1021" s="1"/>
+      <c r="P1021" s="1"/>
+      <c r="Q1021" s="1"/>
+      <c r="R1021" s="1"/>
+      <c r="S1021" s="1"/>
+      <c r="T1021" s="1"/>
+      <c r="U1021" s="1"/>
+      <c r="V1021" s="1"/>
+      <c r="W1021" s="1"/>
+      <c r="X1021" s="1"/>
+      <c r="Y1021" s="1"/>
+    </row>
+    <row r="1022">
+      <c r="A1022" s="1"/>
+      <c r="B1022" s="1"/>
+      <c r="C1022" s="1"/>
+      <c r="D1022" s="1"/>
+      <c r="E1022" s="1"/>
+      <c r="F1022" s="1"/>
+      <c r="G1022" s="1"/>
+      <c r="H1022" s="1"/>
+      <c r="I1022" s="1"/>
+      <c r="J1022" s="1"/>
+      <c r="K1022" s="1"/>
+      <c r="L1022" s="1"/>
+      <c r="M1022" s="1"/>
+      <c r="N1022" s="1"/>
+      <c r="O1022" s="1"/>
+      <c r="P1022" s="1"/>
+      <c r="Q1022" s="1"/>
+      <c r="R1022" s="1"/>
+      <c r="S1022" s="1"/>
+      <c r="T1022" s="1"/>
+      <c r="U1022" s="1"/>
+      <c r="V1022" s="1"/>
+      <c r="W1022" s="1"/>
+      <c r="X1022" s="1"/>
+      <c r="Y1022" s="1"/>
+    </row>
+    <row r="1023">
+      <c r="A1023" s="1"/>
+      <c r="B1023" s="1"/>
+      <c r="C1023" s="1"/>
+      <c r="D1023" s="1"/>
+      <c r="E1023" s="1"/>
+      <c r="F1023" s="1"/>
+      <c r="G1023" s="1"/>
+      <c r="H1023" s="1"/>
+      <c r="I1023" s="1"/>
+      <c r="J1023" s="1"/>
+      <c r="K1023" s="1"/>
+      <c r="L1023" s="1"/>
+      <c r="M1023" s="1"/>
+      <c r="N1023" s="1"/>
+      <c r="O1023" s="1"/>
+      <c r="P1023" s="1"/>
+      <c r="Q1023" s="1"/>
+      <c r="R1023" s="1"/>
+      <c r="S1023" s="1"/>
+      <c r="T1023" s="1"/>
+      <c r="U1023" s="1"/>
+      <c r="V1023" s="1"/>
+      <c r="W1023" s="1"/>
+      <c r="X1023" s="1"/>
+      <c r="Y1023" s="1"/>
+    </row>
+    <row r="1024">
+      <c r="A1024" s="1"/>
+      <c r="B1024" s="1"/>
+      <c r="C1024" s="1"/>
+      <c r="D1024" s="1"/>
+      <c r="E1024" s="1"/>
+      <c r="F1024" s="1"/>
+      <c r="G1024" s="1"/>
+      <c r="H1024" s="1"/>
+      <c r="I1024" s="1"/>
+      <c r="J1024" s="1"/>
+      <c r="K1024" s="1"/>
+      <c r="L1024" s="1"/>
+      <c r="M1024" s="1"/>
+      <c r="N1024" s="1"/>
+      <c r="O1024" s="1"/>
+      <c r="P1024" s="1"/>
+      <c r="Q1024" s="1"/>
+      <c r="R1024" s="1"/>
+      <c r="S1024" s="1"/>
+      <c r="T1024" s="1"/>
+      <c r="U1024" s="1"/>
+      <c r="V1024" s="1"/>
+      <c r="W1024" s="1"/>
+      <c r="X1024" s="1"/>
+      <c r="Y1024" s="1"/>
+    </row>
+    <row r="1025">
+      <c r="A1025" s="1"/>
+      <c r="B1025" s="1"/>
+      <c r="C1025" s="1"/>
+      <c r="D1025" s="1"/>
+      <c r="E1025" s="1"/>
+      <c r="F1025" s="1"/>
+      <c r="G1025" s="1"/>
+      <c r="H1025" s="1"/>
+      <c r="I1025" s="1"/>
+      <c r="J1025" s="1"/>
+      <c r="K1025" s="1"/>
+      <c r="L1025" s="1"/>
+      <c r="M1025" s="1"/>
+      <c r="N1025" s="1"/>
+      <c r="O1025" s="1"/>
+      <c r="P1025" s="1"/>
+      <c r="Q1025" s="1"/>
+      <c r="R1025" s="1"/>
+      <c r="S1025" s="1"/>
+      <c r="T1025" s="1"/>
+      <c r="U1025" s="1"/>
+      <c r="V1025" s="1"/>
+      <c r="W1025" s="1"/>
+      <c r="X1025" s="1"/>
+      <c r="Y1025" s="1"/>
+    </row>
+    <row r="1026">
+      <c r="A1026" s="1"/>
+      <c r="B1026" s="1"/>
+      <c r="C1026" s="1"/>
+      <c r="D1026" s="1"/>
+      <c r="E1026" s="1"/>
+      <c r="F1026" s="1"/>
+      <c r="G1026" s="1"/>
+      <c r="H1026" s="1"/>
+      <c r="I1026" s="1"/>
+      <c r="J1026" s="1"/>
+      <c r="K1026" s="1"/>
+      <c r="L1026" s="1"/>
+      <c r="M1026" s="1"/>
+      <c r="N1026" s="1"/>
+      <c r="O1026" s="1"/>
+      <c r="P1026" s="1"/>
+      <c r="Q1026" s="1"/>
+      <c r="R1026" s="1"/>
+      <c r="S1026" s="1"/>
+      <c r="T1026" s="1"/>
+      <c r="U1026" s="1"/>
+      <c r="V1026" s="1"/>
+      <c r="W1026" s="1"/>
+      <c r="X1026" s="1"/>
+      <c r="Y1026" s="1"/>
+    </row>
+    <row r="1027">
+      <c r="A1027" s="1"/>
+      <c r="B1027" s="1"/>
+      <c r="C1027" s="1"/>
+      <c r="D1027" s="1"/>
+      <c r="E1027" s="1"/>
+      <c r="F1027" s="1"/>
+      <c r="G1027" s="1"/>
+      <c r="H1027" s="1"/>
+      <c r="I1027" s="1"/>
+      <c r="J1027" s="1"/>
+      <c r="K1027" s="1"/>
+      <c r="L1027" s="1"/>
+      <c r="M1027" s="1"/>
+      <c r="N1027" s="1"/>
+      <c r="O1027" s="1"/>
+      <c r="P1027" s="1"/>
+      <c r="Q1027" s="1"/>
+      <c r="R1027" s="1"/>
+      <c r="S1027" s="1"/>
+      <c r="T1027" s="1"/>
+      <c r="U1027" s="1"/>
+      <c r="V1027" s="1"/>
+      <c r="W1027" s="1"/>
+      <c r="X1027" s="1"/>
+      <c r="Y1027" s="1"/>
+    </row>
+    <row r="1028">
+      <c r="A1028" s="1"/>
+      <c r="B1028" s="1"/>
+      <c r="C1028" s="1"/>
+      <c r="D1028" s="1"/>
+      <c r="E1028" s="1"/>
+      <c r="F1028" s="1"/>
+      <c r="G1028" s="1"/>
+      <c r="H1028" s="1"/>
+      <c r="I1028" s="1"/>
+      <c r="J1028" s="1"/>
+      <c r="K1028" s="1"/>
+      <c r="L1028" s="1"/>
+      <c r="M1028" s="1"/>
+      <c r="N1028" s="1"/>
+      <c r="O1028" s="1"/>
+      <c r="P1028" s="1"/>
+      <c r="Q1028" s="1"/>
+      <c r="R1028" s="1"/>
+      <c r="S1028" s="1"/>
+      <c r="T1028" s="1"/>
+      <c r="U1028" s="1"/>
+      <c r="V1028" s="1"/>
+      <c r="W1028" s="1"/>
+      <c r="X1028" s="1"/>
+      <c r="Y1028" s="1"/>
+    </row>
+    <row r="1029">
+      <c r="A1029" s="1"/>
+      <c r="B1029" s="1"/>
+      <c r="C1029" s="1"/>
+      <c r="D1029" s="1"/>
+      <c r="E1029" s="1"/>
+      <c r="F1029" s="1"/>
+      <c r="G1029" s="1"/>
+      <c r="H1029" s="1"/>
+      <c r="I1029" s="1"/>
+      <c r="J1029" s="1"/>
+      <c r="K1029" s="1"/>
+      <c r="L1029" s="1"/>
+      <c r="M1029" s="1"/>
+      <c r="N1029" s="1"/>
+      <c r="O1029" s="1"/>
+      <c r="P1029" s="1"/>
+      <c r="Q1029" s="1"/>
+      <c r="R1029" s="1"/>
+      <c r="S1029" s="1"/>
+      <c r="T1029" s="1"/>
+      <c r="U1029" s="1"/>
+      <c r="V1029" s="1"/>
+      <c r="W1029" s="1"/>
+      <c r="X1029" s="1"/>
+      <c r="Y1029" s="1"/>
+    </row>
+    <row r="1030">
+      <c r="A1030" s="1"/>
+      <c r="B1030" s="1"/>
+      <c r="C1030" s="1"/>
+      <c r="D1030" s="1"/>
+      <c r="E1030" s="1"/>
+      <c r="F1030" s="1"/>
+      <c r="G1030" s="1"/>
+      <c r="H1030" s="1"/>
+      <c r="I1030" s="1"/>
+      <c r="J1030" s="1"/>
+      <c r="K1030" s="1"/>
+      <c r="L1030" s="1"/>
+      <c r="M1030" s="1"/>
+      <c r="N1030" s="1"/>
+      <c r="O1030" s="1"/>
+      <c r="P1030" s="1"/>
+      <c r="Q1030" s="1"/>
+      <c r="R1030" s="1"/>
+      <c r="S1030" s="1"/>
+      <c r="T1030" s="1"/>
+      <c r="U1030" s="1"/>
+      <c r="V1030" s="1"/>
+      <c r="W1030" s="1"/>
+      <c r="X1030" s="1"/>
+      <c r="Y1030" s="1"/>
+    </row>
+    <row r="1031">
+      <c r="A1031" s="1"/>
+      <c r="B1031" s="1"/>
+      <c r="C1031" s="1"/>
+      <c r="D1031" s="1"/>
+      <c r="E1031" s="1"/>
+      <c r="F1031" s="1"/>
+      <c r="G1031" s="1"/>
+      <c r="H1031" s="1"/>
+      <c r="I1031" s="1"/>
+      <c r="J1031" s="1"/>
+      <c r="K1031" s="1"/>
+      <c r="L1031" s="1"/>
+      <c r="M1031" s="1"/>
+      <c r="N1031" s="1"/>
+      <c r="O1031" s="1"/>
+      <c r="P1031" s="1"/>
+      <c r="Q1031" s="1"/>
+      <c r="R1031" s="1"/>
+      <c r="S1031" s="1"/>
+      <c r="T1031" s="1"/>
+      <c r="U1031" s="1"/>
+      <c r="V1031" s="1"/>
+      <c r="W1031" s="1"/>
+      <c r="X1031" s="1"/>
+      <c r="Y1031" s="1"/>
+    </row>
+    <row r="1032">
+      <c r="A1032" s="1"/>
+      <c r="B1032" s="1"/>
+      <c r="C1032" s="1"/>
+      <c r="D1032" s="1"/>
+      <c r="E1032" s="1"/>
+      <c r="F1032" s="1"/>
+      <c r="G1032" s="1"/>
+      <c r="H1032" s="1"/>
+      <c r="I1032" s="1"/>
+      <c r="J1032" s="1"/>
+      <c r="K1032" s="1"/>
+      <c r="L1032" s="1"/>
+      <c r="M1032" s="1"/>
+      <c r="N1032" s="1"/>
+      <c r="O1032" s="1"/>
+      <c r="P1032" s="1"/>
+      <c r="Q1032" s="1"/>
+      <c r="R1032" s="1"/>
+      <c r="S1032" s="1"/>
+      <c r="T1032" s="1"/>
+      <c r="U1032" s="1"/>
+      <c r="V1032" s="1"/>
+      <c r="W1032" s="1"/>
+      <c r="X1032" s="1"/>
+      <c r="Y1032" s="1"/>
+    </row>
+    <row r="1033">
+      <c r="A1033" s="1"/>
+      <c r="B1033" s="1"/>
+      <c r="C1033" s="1"/>
+      <c r="D1033" s="1"/>
+      <c r="E1033" s="1"/>
+      <c r="F1033" s="1"/>
+      <c r="G1033" s="1"/>
+      <c r="H1033" s="1"/>
+      <c r="I1033" s="1"/>
+      <c r="J1033" s="1"/>
+      <c r="K1033" s="1"/>
+      <c r="L1033" s="1"/>
+      <c r="M1033" s="1"/>
+      <c r="N1033" s="1"/>
+      <c r="O1033" s="1"/>
+      <c r="P1033" s="1"/>
+      <c r="Q1033" s="1"/>
+      <c r="R1033" s="1"/>
+      <c r="S1033" s="1"/>
+      <c r="T1033" s="1"/>
+      <c r="U1033" s="1"/>
+      <c r="V1033" s="1"/>
+      <c r="W1033" s="1"/>
+      <c r="X1033" s="1"/>
+      <c r="Y1033" s="1"/>
+    </row>
+    <row r="1034">
+      <c r="A1034" s="1"/>
+      <c r="B1034" s="1"/>
+      <c r="C1034" s="1"/>
+      <c r="D1034" s="1"/>
+      <c r="E1034" s="1"/>
+      <c r="F1034" s="1"/>
+      <c r="G1034" s="1"/>
+      <c r="H1034" s="1"/>
+      <c r="I1034" s="1"/>
+      <c r="J1034" s="1"/>
+      <c r="K1034" s="1"/>
+      <c r="L1034" s="1"/>
+      <c r="M1034" s="1"/>
+      <c r="N1034" s="1"/>
+      <c r="O1034" s="1"/>
+      <c r="P1034" s="1"/>
+      <c r="Q1034" s="1"/>
+      <c r="R1034" s="1"/>
+      <c r="S1034" s="1"/>
+      <c r="T1034" s="1"/>
+      <c r="U1034" s="1"/>
+      <c r="V1034" s="1"/>
+      <c r="W1034" s="1"/>
+      <c r="X1034" s="1"/>
+      <c r="Y1034" s="1"/>
+    </row>
+    <row r="1035">
+      <c r="A1035" s="1"/>
+      <c r="B1035" s="1"/>
+      <c r="C1035" s="1"/>
+      <c r="D1035" s="1"/>
+      <c r="E1035" s="1"/>
+      <c r="F1035" s="1"/>
+      <c r="G1035" s="1"/>
+      <c r="H1035" s="1"/>
+      <c r="I1035" s="1"/>
+      <c r="J1035" s="1"/>
+      <c r="K1035" s="1"/>
+      <c r="L1035" s="1"/>
+      <c r="M1035" s="1"/>
+      <c r="N1035" s="1"/>
+      <c r="O1035" s="1"/>
+      <c r="P1035" s="1"/>
+      <c r="Q1035" s="1"/>
+      <c r="R1035" s="1"/>
+      <c r="S1035" s="1"/>
+      <c r="T1035" s="1"/>
+      <c r="U1035" s="1"/>
+      <c r="V1035" s="1"/>
+      <c r="W1035" s="1"/>
+      <c r="X1035" s="1"/>
+      <c r="Y1035" s="1"/>
+    </row>
+    <row r="1036">
+      <c r="A1036" s="1"/>
+      <c r="B1036" s="1"/>
+      <c r="C1036" s="1"/>
+      <c r="D1036" s="1"/>
+      <c r="E1036" s="1"/>
+      <c r="F1036" s="1"/>
+      <c r="G1036" s="1"/>
+      <c r="H1036" s="1"/>
+      <c r="I1036" s="1"/>
+      <c r="J1036" s="1"/>
+      <c r="K1036" s="1"/>
+      <c r="L1036" s="1"/>
+      <c r="M1036" s="1"/>
+      <c r="N1036" s="1"/>
+      <c r="O1036" s="1"/>
+      <c r="P1036" s="1"/>
+      <c r="Q1036" s="1"/>
+      <c r="R1036" s="1"/>
+      <c r="S1036" s="1"/>
+      <c r="T1036" s="1"/>
+      <c r="U1036" s="1"/>
+      <c r="V1036" s="1"/>
+      <c r="W1036" s="1"/>
+      <c r="X1036" s="1"/>
+      <c r="Y1036" s="1"/>
+    </row>
+    <row r="1037">
+      <c r="A1037" s="1"/>
+      <c r="B1037" s="1"/>
+      <c r="C1037" s="1"/>
+      <c r="D1037" s="1"/>
+      <c r="E1037" s="1"/>
+      <c r="F1037" s="1"/>
+      <c r="G1037" s="1"/>
+      <c r="H1037" s="1"/>
+      <c r="I1037" s="1"/>
+      <c r="J1037" s="1"/>
+      <c r="K1037" s="1"/>
+      <c r="L1037" s="1"/>
+      <c r="M1037" s="1"/>
+      <c r="N1037" s="1"/>
+      <c r="O1037" s="1"/>
+      <c r="P1037" s="1"/>
+      <c r="Q1037" s="1"/>
+      <c r="R1037" s="1"/>
+      <c r="S1037" s="1"/>
+      <c r="T1037" s="1"/>
+      <c r="U1037" s="1"/>
+      <c r="V1037" s="1"/>
+      <c r="W1037" s="1"/>
+      <c r="X1037" s="1"/>
+      <c r="Y1037" s="1"/>
+    </row>
+    <row r="1038">
+      <c r="A1038" s="1"/>
+      <c r="B1038" s="1"/>
+      <c r="C1038" s="1"/>
+      <c r="D1038" s="1"/>
+      <c r="E1038" s="1"/>
+      <c r="F1038" s="1"/>
+      <c r="G1038" s="1"/>
+      <c r="H1038" s="1"/>
+      <c r="I1038" s="1"/>
+      <c r="J1038" s="1"/>
+      <c r="K1038" s="1"/>
+      <c r="L1038" s="1"/>
+      <c r="M1038" s="1"/>
+      <c r="N1038" s="1"/>
+      <c r="O1038" s="1"/>
+      <c r="P1038" s="1"/>
+      <c r="Q1038" s="1"/>
+      <c r="R1038" s="1"/>
+      <c r="S1038" s="1"/>
+      <c r="T1038" s="1"/>
+      <c r="U1038" s="1"/>
+      <c r="V1038" s="1"/>
+      <c r="W1038" s="1"/>
+      <c r="X1038" s="1"/>
+      <c r="Y1038" s="1"/>
+    </row>
+    <row r="1039">
+      <c r="A1039" s="1"/>
+      <c r="B1039" s="1"/>
+      <c r="C1039" s="1"/>
+      <c r="D1039" s="1"/>
+      <c r="E1039" s="1"/>
+      <c r="F1039" s="1"/>
+      <c r="G1039" s="1"/>
+      <c r="H1039" s="1"/>
+      <c r="I1039" s="1"/>
+      <c r="J1039" s="1"/>
+      <c r="K1039" s="1"/>
+      <c r="L1039" s="1"/>
+      <c r="M1039" s="1"/>
+      <c r="N1039" s="1"/>
+      <c r="O1039" s="1"/>
+      <c r="P1039" s="1"/>
+      <c r="Q1039" s="1"/>
+      <c r="R1039" s="1"/>
+      <c r="S1039" s="1"/>
+      <c r="T1039" s="1"/>
+      <c r="U1039" s="1"/>
+      <c r="V1039" s="1"/>
+      <c r="W1039" s="1"/>
+      <c r="X1039" s="1"/>
+      <c r="Y1039" s="1"/>
+    </row>
+    <row r="1040">
+      <c r="A1040" s="1"/>
+      <c r="B1040" s="1"/>
+      <c r="C1040" s="1"/>
+      <c r="D1040" s="1"/>
+      <c r="E1040" s="1"/>
+      <c r="F1040" s="1"/>
+      <c r="G1040" s="1"/>
+      <c r="H1040" s="1"/>
+      <c r="I1040" s="1"/>
+      <c r="J1040" s="1"/>
+      <c r="K1040" s="1"/>
+      <c r="L1040" s="1"/>
+      <c r="M1040" s="1"/>
+      <c r="N1040" s="1"/>
+      <c r="O1040" s="1"/>
+      <c r="P1040" s="1"/>
+      <c r="Q1040" s="1"/>
+      <c r="R1040" s="1"/>
+      <c r="S1040" s="1"/>
+      <c r="T1040" s="1"/>
+      <c r="U1040" s="1"/>
+      <c r="V1040" s="1"/>
+      <c r="W1040" s="1"/>
+      <c r="X1040" s="1"/>
+      <c r="Y1040" s="1"/>
+    </row>
+    <row r="1041">
+      <c r="A1041" s="1"/>
+      <c r="B1041" s="1"/>
+      <c r="C1041" s="1"/>
+      <c r="D1041" s="1"/>
+      <c r="E1041" s="1"/>
+      <c r="F1041" s="1"/>
+      <c r="G1041" s="1"/>
+      <c r="H1041" s="1"/>
+      <c r="I1041" s="1"/>
+      <c r="J1041" s="1"/>
+      <c r="K1041" s="1"/>
+      <c r="L1041" s="1"/>
+      <c r="M1041" s="1"/>
+      <c r="N1041" s="1"/>
+      <c r="O1041" s="1"/>
+      <c r="P1041" s="1"/>
+      <c r="Q1041" s="1"/>
+      <c r="R1041" s="1"/>
+      <c r="S1041" s="1"/>
+      <c r="T1041" s="1"/>
+      <c r="U1041" s="1"/>
+      <c r="V1041" s="1"/>
+      <c r="W1041" s="1"/>
+      <c r="X1041" s="1"/>
+      <c r="Y1041" s="1"/>
+    </row>
+    <row r="1042">
+      <c r="A1042" s="1"/>
+      <c r="B1042" s="1"/>
+      <c r="C1042" s="1"/>
+      <c r="D1042" s="1"/>
+      <c r="E1042" s="1"/>
+      <c r="F1042" s="1"/>
+      <c r="G1042" s="1"/>
+      <c r="H1042" s="1"/>
+      <c r="I1042" s="1"/>
+      <c r="J1042" s="1"/>
+      <c r="K1042" s="1"/>
+      <c r="L1042" s="1"/>
+      <c r="M1042" s="1"/>
+      <c r="N1042" s="1"/>
+      <c r="O1042" s="1"/>
+      <c r="P1042" s="1"/>
+      <c r="Q1042" s="1"/>
+      <c r="R1042" s="1"/>
+      <c r="S1042" s="1"/>
+      <c r="T1042" s="1"/>
+      <c r="U1042" s="1"/>
+      <c r="V1042" s="1"/>
+      <c r="W1042" s="1"/>
+      <c r="X1042" s="1"/>
+      <c r="Y1042" s="1"/>
+    </row>
+    <row r="1043">
+      <c r="A1043" s="1"/>
+      <c r="B1043" s="1"/>
+      <c r="C1043" s="1"/>
+      <c r="D1043" s="1"/>
+      <c r="E1043" s="1"/>
+      <c r="F1043" s="1"/>
+      <c r="G1043" s="1"/>
+      <c r="H1043" s="1"/>
+      <c r="I1043" s="1"/>
+      <c r="J1043" s="1"/>
+      <c r="K1043" s="1"/>
+      <c r="L1043" s="1"/>
+      <c r="M1043" s="1"/>
+      <c r="N1043" s="1"/>
+      <c r="O1043" s="1"/>
+      <c r="P1043" s="1"/>
+      <c r="Q1043" s="1"/>
+      <c r="R1043" s="1"/>
+      <c r="S1043" s="1"/>
+      <c r="T1043" s="1"/>
+      <c r="U1043" s="1"/>
+      <c r="V1043" s="1"/>
+      <c r="W1043" s="1"/>
+      <c r="X1043" s="1"/>
+      <c r="Y1043" s="1"/>
+    </row>
+    <row r="1044">
+      <c r="A1044" s="1"/>
+      <c r="B1044" s="1"/>
+      <c r="C1044" s="1"/>
+      <c r="D1044" s="1"/>
+      <c r="E1044" s="1"/>
+      <c r="F1044" s="1"/>
+      <c r="G1044" s="1"/>
+      <c r="H1044" s="1"/>
+      <c r="I1044" s="1"/>
+      <c r="J1044" s="1"/>
+      <c r="K1044" s="1"/>
+      <c r="L1044" s="1"/>
+      <c r="M1044" s="1"/>
+      <c r="N1044" s="1"/>
+      <c r="O1044" s="1"/>
+      <c r="P1044" s="1"/>
+      <c r="Q1044" s="1"/>
+      <c r="R1044" s="1"/>
+      <c r="S1044" s="1"/>
+      <c r="T1044" s="1"/>
+      <c r="U1044" s="1"/>
+      <c r="V1044" s="1"/>
+      <c r="W1044" s="1"/>
+      <c r="X1044" s="1"/>
+      <c r="Y1044" s="1"/>
+    </row>
+    <row r="1045">
+      <c r="A1045" s="1"/>
+      <c r="B1045" s="1"/>
+      <c r="C1045" s="1"/>
+      <c r="D1045" s="1"/>
+      <c r="E1045" s="1"/>
+      <c r="F1045" s="1"/>
+      <c r="G1045" s="1"/>
+      <c r="H1045" s="1"/>
+      <c r="I1045" s="1"/>
+      <c r="J1045" s="1"/>
+      <c r="K1045" s="1"/>
+      <c r="L1045" s="1"/>
+      <c r="M1045" s="1"/>
+      <c r="N1045" s="1"/>
+      <c r="O1045" s="1"/>
+      <c r="P1045" s="1"/>
+      <c r="Q1045" s="1"/>
+      <c r="R1045" s="1"/>
+      <c r="S1045" s="1"/>
+      <c r="T1045" s="1"/>
+      <c r="U1045" s="1"/>
+      <c r="V1045" s="1"/>
+      <c r="W1045" s="1"/>
+      <c r="X1045" s="1"/>
+      <c r="Y1045" s="1"/>
+    </row>
+    <row r="1046">
+      <c r="A1046" s="1"/>
+      <c r="B1046" s="1"/>
+      <c r="C1046" s="1"/>
+      <c r="D1046" s="1"/>
+      <c r="E1046" s="1"/>
+      <c r="F1046" s="1"/>
+      <c r="G1046" s="1"/>
+      <c r="H1046" s="1"/>
+      <c r="I1046" s="1"/>
+      <c r="J1046" s="1"/>
+      <c r="K1046" s="1"/>
+      <c r="L1046" s="1"/>
+      <c r="M1046" s="1"/>
+      <c r="N1046" s="1"/>
+      <c r="O1046" s="1"/>
+      <c r="P1046" s="1"/>
+      <c r="Q1046" s="1"/>
+      <c r="R1046" s="1"/>
+      <c r="S1046" s="1"/>
+      <c r="T1046" s="1"/>
+      <c r="U1046" s="1"/>
+      <c r="V1046" s="1"/>
+      <c r="W1046" s="1"/>
+      <c r="X1046" s="1"/>
+      <c r="Y1046" s="1"/>
+    </row>
+    <row r="1047">
+      <c r="A1047" s="1"/>
+      <c r="B1047" s="1"/>
+      <c r="C1047" s="1"/>
+      <c r="D1047" s="1"/>
+      <c r="E1047" s="1"/>
+      <c r="F1047" s="1"/>
+      <c r="G1047" s="1"/>
+      <c r="H1047" s="1"/>
+      <c r="I1047" s="1"/>
+      <c r="J1047" s="1"/>
+      <c r="K1047" s="1"/>
+      <c r="L1047" s="1"/>
+      <c r="M1047" s="1"/>
+      <c r="N1047" s="1"/>
+      <c r="O1047" s="1"/>
+      <c r="P1047" s="1"/>
+      <c r="Q1047" s="1"/>
+      <c r="R1047" s="1"/>
+      <c r="S1047" s="1"/>
+      <c r="T1047" s="1"/>
+      <c r="U1047" s="1"/>
+      <c r="V1047" s="1"/>
+      <c r="W1047" s="1"/>
+      <c r="X1047" s="1"/>
+      <c r="Y1047" s="1"/>
+    </row>
+    <row r="1048">
+      <c r="A1048" s="1"/>
+      <c r="B1048" s="1"/>
+      <c r="C1048" s="1"/>
+      <c r="D1048" s="1"/>
+      <c r="E1048" s="1"/>
+      <c r="F1048" s="1"/>
+      <c r="G1048" s="1"/>
+      <c r="H1048" s="1"/>
+      <c r="I1048" s="1"/>
+      <c r="J1048" s="1"/>
+      <c r="K1048" s="1"/>
+      <c r="L1048" s="1"/>
+      <c r="M1048" s="1"/>
+      <c r="N1048" s="1"/>
+      <c r="O1048" s="1"/>
+      <c r="P1048" s="1"/>
+      <c r="Q1048" s="1"/>
+      <c r="R1048" s="1"/>
+      <c r="S1048" s="1"/>
+      <c r="T1048" s="1"/>
+      <c r="U1048" s="1"/>
+      <c r="V1048" s="1"/>
+      <c r="W1048" s="1"/>
+      <c r="X1048" s="1"/>
+      <c r="Y1048" s="1"/>
+    </row>
+    <row r="1049">
+      <c r="A1049" s="1"/>
+      <c r="B1049" s="1"/>
+      <c r="C1049" s="1"/>
+      <c r="D1049" s="1"/>
+      <c r="E1049" s="1"/>
+      <c r="F1049" s="1"/>
+      <c r="G1049" s="1"/>
+      <c r="H1049" s="1"/>
+      <c r="I1049" s="1"/>
+      <c r="J1049" s="1"/>
+      <c r="K1049" s="1"/>
+      <c r="L1049" s="1"/>
+      <c r="M1049" s="1"/>
+      <c r="N1049" s="1"/>
+      <c r="O1049" s="1"/>
+      <c r="P1049" s="1"/>
+      <c r="Q1049" s="1"/>
+      <c r="R1049" s="1"/>
+      <c r="S1049" s="1"/>
+      <c r="T1049" s="1"/>
+      <c r="U1049" s="1"/>
+      <c r="V1049" s="1"/>
+      <c r="W1049" s="1"/>
+      <c r="X1049" s="1"/>
+      <c r="Y1049" s="1"/>
+    </row>
+    <row r="1050">
+      <c r="A1050" s="1"/>
+      <c r="B1050" s="1"/>
+      <c r="C1050" s="1"/>
+      <c r="D1050" s="1"/>
+      <c r="E1050" s="1"/>
+      <c r="F1050" s="1"/>
+      <c r="G1050" s="1"/>
+      <c r="H1050" s="1"/>
+      <c r="I1050" s="1"/>
+      <c r="J1050" s="1"/>
+      <c r="K1050" s="1"/>
+      <c r="L1050" s="1"/>
+      <c r="M1050" s="1"/>
+      <c r="N1050" s="1"/>
+      <c r="O1050" s="1"/>
+      <c r="P1050" s="1"/>
+      <c r="Q1050" s="1"/>
+      <c r="R1050" s="1"/>
+      <c r="S1050" s="1"/>
+      <c r="T1050" s="1"/>
+      <c r="U1050" s="1"/>
+      <c r="V1050" s="1"/>
+      <c r="W1050" s="1"/>
+      <c r="X1050" s="1"/>
+      <c r="Y1050" s="1"/>
+    </row>
+    <row r="1051">
+      <c r="A1051" s="1"/>
+      <c r="B1051" s="1"/>
+      <c r="C1051" s="1"/>
+      <c r="D1051" s="1"/>
+      <c r="E1051" s="1"/>
+      <c r="F1051" s="1"/>
+      <c r="G1051" s="1"/>
+      <c r="H1051" s="1"/>
+      <c r="I1051" s="1"/>
+      <c r="J1051" s="1"/>
+      <c r="K1051" s="1"/>
+      <c r="L1051" s="1"/>
+      <c r="M1051" s="1"/>
+      <c r="N1051" s="1"/>
+      <c r="O1051" s="1"/>
+      <c r="P1051" s="1"/>
+      <c r="Q1051" s="1"/>
+      <c r="R1051" s="1"/>
+      <c r="S1051" s="1"/>
+      <c r="T1051" s="1"/>
+      <c r="U1051" s="1"/>
+      <c r="V1051" s="1"/>
+      <c r="W1051" s="1"/>
+      <c r="X1051" s="1"/>
+      <c r="Y1051" s="1"/>
+    </row>
+    <row r="1052">
+      <c r="A1052" s="1"/>
+      <c r="B1052" s="1"/>
+      <c r="C1052" s="1"/>
+      <c r="D1052" s="1"/>
+      <c r="E1052" s="1"/>
+      <c r="F1052" s="1"/>
+      <c r="G1052" s="1"/>
+      <c r="H1052" s="1"/>
+      <c r="I1052" s="1"/>
+      <c r="J1052" s="1"/>
+      <c r="K1052" s="1"/>
+      <c r="L1052" s="1"/>
+      <c r="M1052" s="1"/>
+      <c r="N1052" s="1"/>
+      <c r="O1052" s="1"/>
+      <c r="P1052" s="1"/>
+      <c r="Q1052" s="1"/>
+      <c r="R1052" s="1"/>
+      <c r="S1052" s="1"/>
+      <c r="T1052" s="1"/>
+      <c r="U1052" s="1"/>
+      <c r="V1052" s="1"/>
+      <c r="W1052" s="1"/>
+      <c r="X1052" s="1"/>
+      <c r="Y1052" s="1"/>
+    </row>
+    <row r="1053">
+      <c r="A1053" s="1"/>
+      <c r="B1053" s="1"/>
+      <c r="C1053" s="1"/>
+      <c r="D1053" s="1"/>
+      <c r="E1053" s="1"/>
+      <c r="F1053" s="1"/>
+      <c r="G1053" s="1"/>
+      <c r="H1053" s="1"/>
+      <c r="I1053" s="1"/>
+      <c r="J1053" s="1"/>
+      <c r="K1053" s="1"/>
+      <c r="L1053" s="1"/>
+      <c r="M1053" s="1"/>
+      <c r="N1053" s="1"/>
+      <c r="O1053" s="1"/>
+      <c r="P1053" s="1"/>
+      <c r="Q1053" s="1"/>
+      <c r="R1053" s="1"/>
+      <c r="S1053" s="1"/>
+      <c r="T1053" s="1"/>
+      <c r="U1053" s="1"/>
+      <c r="V1053" s="1"/>
+      <c r="W1053" s="1"/>
+      <c r="X1053" s="1"/>
+      <c r="Y1053" s="1"/>
+    </row>
+    <row r="1054">
+      <c r="A1054" s="1"/>
+      <c r="B1054" s="1"/>
+      <c r="C1054" s="1"/>
+      <c r="D1054" s="1"/>
+      <c r="E1054" s="1"/>
+      <c r="F1054" s="1"/>
+      <c r="G1054" s="1"/>
+      <c r="H1054" s="1"/>
+      <c r="I1054" s="1"/>
+      <c r="J1054" s="1"/>
+      <c r="K1054" s="1"/>
+      <c r="L1054" s="1"/>
+      <c r="M1054" s="1"/>
+      <c r="N1054" s="1"/>
+      <c r="O1054" s="1"/>
+      <c r="P1054" s="1"/>
+      <c r="Q1054" s="1"/>
+      <c r="R1054" s="1"/>
+      <c r="S1054" s="1"/>
+      <c r="T1054" s="1"/>
+      <c r="U1054" s="1"/>
+      <c r="V1054" s="1"/>
+      <c r="W1054" s="1"/>
+      <c r="X1054" s="1"/>
+      <c r="Y1054" s="1"/>
+    </row>
+    <row r="1055">
+      <c r="A1055" s="1"/>
+      <c r="B1055" s="1"/>
+      <c r="C1055" s="1"/>
+      <c r="D1055" s="1"/>
+      <c r="E1055" s="1"/>
+      <c r="F1055" s="1"/>
+      <c r="G1055" s="1"/>
+      <c r="H1055" s="1"/>
+      <c r="I1055" s="1"/>
+      <c r="J1055" s="1"/>
+      <c r="K1055" s="1"/>
+      <c r="L1055" s="1"/>
+      <c r="M1055" s="1"/>
+      <c r="N1055" s="1"/>
+      <c r="O1055" s="1"/>
+      <c r="P1055" s="1"/>
+      <c r="Q1055" s="1"/>
+      <c r="R1055" s="1"/>
+      <c r="S1055" s="1"/>
+      <c r="T1055" s="1"/>
+      <c r="U1055" s="1"/>
+      <c r="V1055" s="1"/>
+      <c r="W1055" s="1"/>
+      <c r="X1055" s="1"/>
+      <c r="Y1055" s="1"/>
+    </row>
+    <row r="1056">
+      <c r="A1056" s="1"/>
+      <c r="B1056" s="1"/>
+      <c r="C1056" s="1"/>
+      <c r="D1056" s="1"/>
+      <c r="E1056" s="1"/>
+      <c r="F1056" s="1"/>
+      <c r="G1056" s="1"/>
+      <c r="H1056" s="1"/>
+      <c r="I1056" s="1"/>
+      <c r="J1056" s="1"/>
+      <c r="K1056" s="1"/>
+      <c r="L1056" s="1"/>
+      <c r="M1056" s="1"/>
+      <c r="N1056" s="1"/>
+      <c r="O1056" s="1"/>
+      <c r="P1056" s="1"/>
+      <c r="Q1056" s="1"/>
+      <c r="R1056" s="1"/>
+      <c r="S1056" s="1"/>
+      <c r="T1056" s="1"/>
+      <c r="U1056" s="1"/>
+      <c r="V1056" s="1"/>
+      <c r="W1056" s="1"/>
+      <c r="X1056" s="1"/>
+      <c r="Y1056" s="1"/>
+    </row>
+    <row r="1057">
+      <c r="A1057" s="1"/>
+      <c r="B1057" s="1"/>
+      <c r="C1057" s="1"/>
+      <c r="D1057" s="1"/>
+      <c r="E1057" s="1"/>
+      <c r="F1057" s="1"/>
+      <c r="G1057" s="1"/>
+      <c r="H1057" s="1"/>
+      <c r="I1057" s="1"/>
+      <c r="J1057" s="1"/>
+      <c r="K1057" s="1"/>
+      <c r="L1057" s="1"/>
+      <c r="M1057" s="1"/>
+      <c r="N1057" s="1"/>
+      <c r="O1057" s="1"/>
+      <c r="P1057" s="1"/>
+      <c r="Q1057" s="1"/>
+      <c r="R1057" s="1"/>
+      <c r="S1057" s="1"/>
+      <c r="T1057" s="1"/>
+      <c r="U1057" s="1"/>
+      <c r="V1057" s="1"/>
+      <c r="W1057" s="1"/>
+      <c r="X1057" s="1"/>
+      <c r="Y1057" s="1"/>
+    </row>
+    <row r="1058">
+      <c r="A1058" s="1"/>
+      <c r="B1058" s="1"/>
+      <c r="C1058" s="1"/>
+      <c r="D1058" s="1"/>
+      <c r="E1058" s="1"/>
+      <c r="F1058" s="1"/>
+      <c r="G1058" s="1"/>
+      <c r="H1058" s="1"/>
+      <c r="I1058" s="1"/>
+      <c r="J1058" s="1"/>
+      <c r="K1058" s="1"/>
+      <c r="L1058" s="1"/>
+      <c r="M1058" s="1"/>
+      <c r="N1058" s="1"/>
+      <c r="O1058" s="1"/>
+      <c r="P1058" s="1"/>
+      <c r="Q1058" s="1"/>
+      <c r="R1058" s="1"/>
+      <c r="S1058" s="1"/>
+      <c r="T1058" s="1"/>
+      <c r="U1058" s="1"/>
+      <c r="V1058" s="1"/>
+      <c r="W1058" s="1"/>
+      <c r="X1058" s="1"/>
+      <c r="Y1058" s="1"/>
+    </row>
+    <row r="1059">
+      <c r="A1059" s="1"/>
+      <c r="B1059" s="1"/>
+      <c r="C1059" s="1"/>
+      <c r="D1059" s="1"/>
+      <c r="E1059" s="1"/>
+      <c r="F1059" s="1"/>
+      <c r="G1059" s="1"/>
+      <c r="H1059" s="1"/>
+      <c r="I1059" s="1"/>
+      <c r="J1059" s="1"/>
+      <c r="K1059" s="1"/>
+      <c r="L1059" s="1"/>
+      <c r="M1059" s="1"/>
+      <c r="N1059" s="1"/>
+      <c r="O1059" s="1"/>
+      <c r="P1059" s="1"/>
+      <c r="Q1059" s="1"/>
+      <c r="R1059" s="1"/>
+      <c r="S1059" s="1"/>
+      <c r="T1059" s="1"/>
+      <c r="U1059" s="1"/>
+      <c r="V1059" s="1"/>
+      <c r="W1059" s="1"/>
+      <c r="X1059" s="1"/>
+      <c r="Y1059" s="1"/>
+    </row>
+    <row r="1060">
+      <c r="A1060" s="1"/>
+      <c r="B1060" s="1"/>
+      <c r="C1060" s="1"/>
+      <c r="D1060" s="1"/>
+      <c r="E1060" s="1"/>
+      <c r="F1060" s="1"/>
+      <c r="G1060" s="1"/>
+      <c r="H1060" s="1"/>
+      <c r="I1060" s="1"/>
+      <c r="J1060" s="1"/>
+      <c r="K1060" s="1"/>
+      <c r="L1060" s="1"/>
+      <c r="M1060" s="1"/>
+      <c r="N1060" s="1"/>
+      <c r="O1060" s="1"/>
+      <c r="P1060" s="1"/>
+      <c r="Q1060" s="1"/>
+      <c r="R1060" s="1"/>
+      <c r="S1060" s="1"/>
+      <c r="T1060" s="1"/>
+      <c r="U1060" s="1"/>
+      <c r="V1060" s="1"/>
+      <c r="W1060" s="1"/>
+      <c r="X1060" s="1"/>
+      <c r="Y1060" s="1"/>
+    </row>
+    <row r="1061">
+      <c r="A1061" s="1"/>
+      <c r="B1061" s="1"/>
+      <c r="C1061" s="1"/>
+      <c r="D1061" s="1"/>
+      <c r="E1061" s="1"/>
+      <c r="F1061" s="1"/>
+      <c r="G1061" s="1"/>
+      <c r="H1061" s="1"/>
+      <c r="I1061" s="1"/>
+      <c r="J1061" s="1"/>
+      <c r="K1061" s="1"/>
+      <c r="L1061" s="1"/>
+      <c r="M1061" s="1"/>
+      <c r="N1061" s="1"/>
+      <c r="O1061" s="1"/>
+      <c r="P1061" s="1"/>
+      <c r="Q1061" s="1"/>
+      <c r="R1061" s="1"/>
+      <c r="S1061" s="1"/>
+      <c r="T1061" s="1"/>
+      <c r="U1061" s="1"/>
+      <c r="V1061" s="1"/>
+      <c r="W1061" s="1"/>
+      <c r="X1061" s="1"/>
+      <c r="Y1061" s="1"/>
+    </row>
+    <row r="1062">
+      <c r="A1062" s="1"/>
+      <c r="B1062" s="1"/>
+      <c r="C1062" s="1"/>
+      <c r="D1062" s="1"/>
+      <c r="E1062" s="1"/>
+      <c r="F1062" s="1"/>
+      <c r="G1062" s="1"/>
+      <c r="H1062" s="1"/>
+      <c r="I1062" s="1"/>
+      <c r="J1062" s="1"/>
+      <c r="K1062" s="1"/>
+      <c r="L1062" s="1"/>
+      <c r="M1062" s="1"/>
+      <c r="N1062" s="1"/>
+      <c r="O1062" s="1"/>
+      <c r="P1062" s="1"/>
+      <c r="Q1062" s="1"/>
+      <c r="R1062" s="1"/>
+      <c r="S1062" s="1"/>
+      <c r="T1062" s="1"/>
+      <c r="U1062" s="1"/>
+      <c r="V1062" s="1"/>
+      <c r="W1062" s="1"/>
+      <c r="X1062" s="1"/>
+      <c r="Y1062" s="1"/>
+    </row>
+    <row r="1063">
+      <c r="A1063" s="1"/>
+      <c r="B1063" s="1"/>
+      <c r="C1063" s="1"/>
+      <c r="D1063" s="1"/>
+      <c r="E1063" s="1"/>
+      <c r="F1063" s="1"/>
+      <c r="G1063" s="1"/>
+      <c r="H1063" s="1"/>
+      <c r="I1063" s="1"/>
+      <c r="J1063" s="1"/>
+      <c r="K1063" s="1"/>
+      <c r="L1063" s="1"/>
+      <c r="M1063" s="1"/>
+      <c r="N1063" s="1"/>
+      <c r="O1063" s="1"/>
+      <c r="P1063" s="1"/>
+      <c r="Q1063" s="1"/>
+      <c r="R1063" s="1"/>
+      <c r="S1063" s="1"/>
+      <c r="T1063" s="1"/>
+      <c r="U1063" s="1"/>
+      <c r="V1063" s="1"/>
+      <c r="W1063" s="1"/>
+      <c r="X1063" s="1"/>
+      <c r="Y1063" s="1"/>
+    </row>
+    <row r="1064">
+      <c r="A1064" s="1"/>
+      <c r="B1064" s="1"/>
+      <c r="C1064" s="1"/>
+      <c r="D1064" s="1"/>
+      <c r="E1064" s="1"/>
+      <c r="F1064" s="1"/>
+      <c r="G1064" s="1"/>
+      <c r="H1064" s="1"/>
+      <c r="I1064" s="1"/>
+      <c r="J1064" s="1"/>
+      <c r="K1064" s="1"/>
+      <c r="L1064" s="1"/>
+      <c r="M1064" s="1"/>
+      <c r="N1064" s="1"/>
+      <c r="O1064" s="1"/>
+      <c r="P1064" s="1"/>
+      <c r="Q1064" s="1"/>
+      <c r="R1064" s="1"/>
+      <c r="S1064" s="1"/>
+      <c r="T1064" s="1"/>
+      <c r="U1064" s="1"/>
+      <c r="V1064" s="1"/>
+      <c r="W1064" s="1"/>
+      <c r="X1064" s="1"/>
+      <c r="Y1064" s="1"/>
+    </row>
+    <row r="1065">
+      <c r="A1065" s="1"/>
+      <c r="B1065" s="1"/>
+      <c r="C1065" s="1"/>
+      <c r="D1065" s="1"/>
+      <c r="E1065" s="1"/>
+      <c r="F1065" s="1"/>
+      <c r="G1065" s="1"/>
+      <c r="H1065" s="1"/>
+      <c r="I1065" s="1"/>
+      <c r="J1065" s="1"/>
+      <c r="K1065" s="1"/>
+      <c r="L1065" s="1"/>
+      <c r="M1065" s="1"/>
+      <c r="N1065" s="1"/>
+      <c r="O1065" s="1"/>
+      <c r="P1065" s="1"/>
+      <c r="Q1065" s="1"/>
+      <c r="R1065" s="1"/>
+      <c r="S1065" s="1"/>
+      <c r="T1065" s="1"/>
+      <c r="U1065" s="1"/>
+      <c r="V1065" s="1"/>
+      <c r="W1065" s="1"/>
+      <c r="X1065" s="1"/>
+      <c r="Y1065" s="1"/>
+    </row>
+    <row r="1066">
+      <c r="A1066" s="1"/>
+      <c r="B1066" s="1"/>
+      <c r="C1066" s="1"/>
+      <c r="D1066" s="1"/>
+      <c r="E1066" s="1"/>
+      <c r="F1066" s="1"/>
+      <c r="G1066" s="1"/>
+      <c r="H1066" s="1"/>
+      <c r="I1066" s="1"/>
+      <c r="J1066" s="1"/>
+      <c r="K1066" s="1"/>
+      <c r="L1066" s="1"/>
+      <c r="M1066" s="1"/>
+      <c r="N1066" s="1"/>
+      <c r="O1066" s="1"/>
+      <c r="P1066" s="1"/>
+      <c r="Q1066" s="1"/>
+      <c r="R1066" s="1"/>
+      <c r="S1066" s="1"/>
+      <c r="T1066" s="1"/>
+      <c r="U1066" s="1"/>
+      <c r="V1066" s="1"/>
+      <c r="W1066" s="1"/>
+      <c r="X1066" s="1"/>
+      <c r="Y1066" s="1"/>
+    </row>
+    <row r="1067">
+      <c r="A1067" s="1"/>
+      <c r="B1067" s="1"/>
+      <c r="C1067" s="1"/>
+      <c r="D1067" s="1"/>
+      <c r="E1067" s="1"/>
+      <c r="F1067" s="1"/>
+      <c r="G1067" s="1"/>
+      <c r="H1067" s="1"/>
+      <c r="I1067" s="1"/>
+      <c r="J1067" s="1"/>
+      <c r="K1067" s="1"/>
+      <c r="L1067" s="1"/>
+      <c r="M1067" s="1"/>
+      <c r="N1067" s="1"/>
+      <c r="O1067" s="1"/>
+      <c r="P1067" s="1"/>
+      <c r="Q1067" s="1"/>
+      <c r="R1067" s="1"/>
+      <c r="S1067" s="1"/>
+      <c r="T1067" s="1"/>
+      <c r="U1067" s="1"/>
+      <c r="V1067" s="1"/>
+      <c r="W1067" s="1"/>
+      <c r="X1067" s="1"/>
+      <c r="Y1067" s="1"/>
+    </row>
+    <row r="1068">
+      <c r="A1068" s="1"/>
+      <c r="B1068" s="1"/>
+      <c r="C1068" s="1"/>
+      <c r="D1068" s="1"/>
+      <c r="E1068" s="1"/>
+      <c r="F1068" s="1"/>
+      <c r="G1068" s="1"/>
+      <c r="H1068" s="1"/>
+      <c r="I1068" s="1"/>
+      <c r="J1068" s="1"/>
+      <c r="K1068" s="1"/>
+      <c r="L1068" s="1"/>
+      <c r="M1068" s="1"/>
+      <c r="N1068" s="1"/>
+      <c r="O1068" s="1"/>
+      <c r="P1068" s="1"/>
+      <c r="Q1068" s="1"/>
+      <c r="R1068" s="1"/>
+      <c r="S1068" s="1"/>
+      <c r="T1068" s="1"/>
+      <c r="U1068" s="1"/>
+      <c r="V1068" s="1"/>
+      <c r="W1068" s="1"/>
+      <c r="X1068" s="1"/>
+      <c r="Y1068" s="1"/>
+    </row>
+    <row r="1069">
+      <c r="A1069" s="1"/>
+      <c r="B1069" s="1"/>
+      <c r="C1069" s="1"/>
+      <c r="D1069" s="1"/>
+      <c r="E1069" s="1"/>
+      <c r="F1069" s="1"/>
+      <c r="G1069" s="1"/>
+      <c r="H1069" s="1"/>
+      <c r="I1069" s="1"/>
+      <c r="J1069" s="1"/>
+      <c r="K1069" s="1"/>
+      <c r="L1069" s="1"/>
+      <c r="M1069" s="1"/>
+      <c r="N1069" s="1"/>
+      <c r="O1069" s="1"/>
+      <c r="P1069" s="1"/>
+      <c r="Q1069" s="1"/>
+      <c r="R1069" s="1"/>
+      <c r="S1069" s="1"/>
+      <c r="T1069" s="1"/>
+      <c r="U1069" s="1"/>
+      <c r="V1069" s="1"/>
+      <c r="W1069" s="1"/>
+      <c r="X1069" s="1"/>
+      <c r="Y1069" s="1"/>
+    </row>
+    <row r="1070">
+      <c r="A1070" s="1"/>
+      <c r="B1070" s="1"/>
+      <c r="C1070" s="1"/>
+      <c r="D1070" s="1"/>
+      <c r="E1070" s="1"/>
+      <c r="F1070" s="1"/>
+      <c r="G1070" s="1"/>
+      <c r="H1070" s="1"/>
+      <c r="I1070" s="1"/>
+      <c r="J1070" s="1"/>
+      <c r="K1070" s="1"/>
+      <c r="L1070" s="1"/>
+      <c r="M1070" s="1"/>
+      <c r="N1070" s="1"/>
+      <c r="O1070" s="1"/>
+      <c r="P1070" s="1"/>
+      <c r="Q1070" s="1"/>
+      <c r="R1070" s="1"/>
+      <c r="S1070" s="1"/>
+      <c r="T1070" s="1"/>
+      <c r="U1070" s="1"/>
+      <c r="V1070" s="1"/>
+      <c r="W1070" s="1"/>
+      <c r="X1070" s="1"/>
+      <c r="Y1070" s="1"/>
+    </row>
+    <row r="1071">
+      <c r="A1071" s="1"/>
+      <c r="B1071" s="1"/>
+      <c r="C1071" s="1"/>
+      <c r="D1071" s="1"/>
+      <c r="E1071" s="1"/>
+      <c r="F1071" s="1"/>
+      <c r="G1071" s="1"/>
+      <c r="H1071" s="1"/>
+      <c r="I1071" s="1"/>
+      <c r="J1071" s="1"/>
+      <c r="K1071" s="1"/>
+      <c r="L1071" s="1"/>
+      <c r="M1071" s="1"/>
+      <c r="N1071" s="1"/>
+      <c r="O1071" s="1"/>
+      <c r="P1071" s="1"/>
+      <c r="Q1071" s="1"/>
+      <c r="R1071" s="1"/>
+      <c r="S1071" s="1"/>
+      <c r="T1071" s="1"/>
+      <c r="U1071" s="1"/>
+      <c r="V1071" s="1"/>
+      <c r="W1071" s="1"/>
+      <c r="X1071" s="1"/>
+      <c r="Y1071" s="1"/>
+    </row>
+    <row r="1072">
+      <c r="A1072" s="1"/>
+      <c r="B1072" s="1"/>
+      <c r="C1072" s="1"/>
+      <c r="D1072" s="1"/>
+      <c r="E1072" s="1"/>
+      <c r="F1072" s="1"/>
+      <c r="G1072" s="1"/>
+      <c r="H1072" s="1"/>
+      <c r="I1072" s="1"/>
+      <c r="J1072" s="1"/>
+      <c r="K1072" s="1"/>
+      <c r="L1072" s="1"/>
+      <c r="M1072" s="1"/>
+      <c r="N1072" s="1"/>
+      <c r="O1072" s="1"/>
+      <c r="P1072" s="1"/>
+      <c r="Q1072" s="1"/>
+      <c r="R1072" s="1"/>
+      <c r="S1072" s="1"/>
+      <c r="T1072" s="1"/>
+      <c r="U1072" s="1"/>
+      <c r="V1072" s="1"/>
+      <c r="W1072" s="1"/>
+      <c r="X1072" s="1"/>
+      <c r="Y1072" s="1"/>
+    </row>
+    <row r="1073">
+      <c r="A1073" s="1"/>
+      <c r="B1073" s="1"/>
+      <c r="C1073" s="1"/>
+      <c r="D1073" s="1"/>
+      <c r="E1073" s="1"/>
+      <c r="F1073" s="1"/>
+      <c r="G1073" s="1"/>
+      <c r="H1073" s="1"/>
+      <c r="I1073" s="1"/>
+      <c r="J1073" s="1"/>
+      <c r="K1073" s="1"/>
+      <c r="L1073" s="1"/>
+      <c r="M1073" s="1"/>
+      <c r="N1073" s="1"/>
+      <c r="O1073" s="1"/>
+      <c r="P1073" s="1"/>
+      <c r="Q1073" s="1"/>
+      <c r="R1073" s="1"/>
+      <c r="S1073" s="1"/>
+      <c r="T1073" s="1"/>
+      <c r="U1073" s="1"/>
+      <c r="V1073" s="1"/>
+      <c r="W1073" s="1"/>
+      <c r="X1073" s="1"/>
+      <c r="Y1073" s="1"/>
+    </row>
+    <row r="1074">
+      <c r="A1074" s="1"/>
+      <c r="B1074" s="1"/>
+      <c r="C1074" s="1"/>
+      <c r="D1074" s="1"/>
+      <c r="E1074" s="1"/>
+      <c r="F1074" s="1"/>
+      <c r="G1074" s="1"/>
+      <c r="H1074" s="1"/>
+      <c r="I1074" s="1"/>
+      <c r="J1074" s="1"/>
+      <c r="K1074" s="1"/>
+      <c r="L1074" s="1"/>
+      <c r="M1074" s="1"/>
+      <c r="N1074" s="1"/>
+      <c r="O1074" s="1"/>
+      <c r="P1074" s="1"/>
+      <c r="Q1074" s="1"/>
+      <c r="R1074" s="1"/>
+      <c r="S1074" s="1"/>
+      <c r="T1074" s="1"/>
+      <c r="U1074" s="1"/>
+      <c r="V1074" s="1"/>
+      <c r="W1074" s="1"/>
+      <c r="X1074" s="1"/>
+      <c r="Y1074" s="1"/>
+    </row>
+    <row r="1075">
+      <c r="A1075" s="1"/>
+      <c r="B1075" s="1"/>
+      <c r="C1075" s="1"/>
+      <c r="D1075" s="1"/>
+      <c r="E1075" s="1"/>
+      <c r="F1075" s="1"/>
+      <c r="G1075" s="1"/>
+      <c r="H1075" s="1"/>
+      <c r="I1075" s="1"/>
+      <c r="J1075" s="1"/>
+      <c r="K1075" s="1"/>
+      <c r="L1075" s="1"/>
+      <c r="M1075" s="1"/>
+      <c r="N1075" s="1"/>
+      <c r="O1075" s="1"/>
+      <c r="P1075" s="1"/>
+      <c r="Q1075" s="1"/>
+      <c r="R1075" s="1"/>
+      <c r="S1075" s="1"/>
+      <c r="T1075" s="1"/>
+      <c r="U1075" s="1"/>
+      <c r="V1075" s="1"/>
+      <c r="W1075" s="1"/>
+      <c r="X1075" s="1"/>
+      <c r="Y1075" s="1"/>
+    </row>
+    <row r="1076">
+      <c r="A1076" s="1"/>
+      <c r="B1076" s="1"/>
+      <c r="C1076" s="1"/>
+      <c r="D1076" s="1"/>
+      <c r="E1076" s="1"/>
+      <c r="F1076" s="1"/>
+      <c r="G1076" s="1"/>
+      <c r="H1076" s="1"/>
+      <c r="I1076" s="1"/>
+      <c r="J1076" s="1"/>
+      <c r="K1076" s="1"/>
+      <c r="L1076" s="1"/>
+      <c r="M1076" s="1"/>
+      <c r="N1076" s="1"/>
+      <c r="O1076" s="1"/>
+      <c r="P1076" s="1"/>
+      <c r="Q1076" s="1"/>
+      <c r="R1076" s="1"/>
+      <c r="S1076" s="1"/>
+      <c r="T1076" s="1"/>
+      <c r="U1076" s="1"/>
+      <c r="V1076" s="1"/>
+      <c r="W1076" s="1"/>
+      <c r="X1076" s="1"/>
+      <c r="Y1076" s="1"/>
+    </row>
+    <row r="1077">
+      <c r="A1077" s="1"/>
+      <c r="B1077" s="1"/>
+      <c r="C1077" s="1"/>
+      <c r="D1077" s="1"/>
+      <c r="E1077" s="1"/>
+      <c r="F1077" s="1"/>
+      <c r="G1077" s="1"/>
+      <c r="H1077" s="1"/>
+      <c r="I1077" s="1"/>
+      <c r="J1077" s="1"/>
+      <c r="K1077" s="1"/>
+      <c r="L1077" s="1"/>
+      <c r="M1077" s="1"/>
+      <c r="N1077" s="1"/>
+      <c r="O1077" s="1"/>
+      <c r="P1077" s="1"/>
+      <c r="Q1077" s="1"/>
+      <c r="R1077" s="1"/>
+      <c r="S1077" s="1"/>
+      <c r="T1077" s="1"/>
+      <c r="U1077" s="1"/>
+      <c r="V1077" s="1"/>
+      <c r="W1077" s="1"/>
+      <c r="X1077" s="1"/>
+      <c r="Y1077" s="1"/>
+    </row>
+    <row r="1078">
+      <c r="A1078" s="1"/>
+      <c r="B1078" s="1"/>
+      <c r="C1078" s="1"/>
+      <c r="D1078" s="1"/>
+      <c r="E1078" s="1"/>
+      <c r="F1078" s="1"/>
+      <c r="G1078" s="1"/>
+      <c r="H1078" s="1"/>
+      <c r="I1078" s="1"/>
+      <c r="J1078" s="1"/>
+      <c r="K1078" s="1"/>
+      <c r="L1078" s="1"/>
+      <c r="M1078" s="1"/>
+      <c r="N1078" s="1"/>
+      <c r="O1078" s="1"/>
+      <c r="P1078" s="1"/>
+      <c r="Q1078" s="1"/>
+      <c r="R1078" s="1"/>
+      <c r="S1078" s="1"/>
+      <c r="T1078" s="1"/>
+      <c r="U1078" s="1"/>
+      <c r="V1078" s="1"/>
+      <c r="W1078" s="1"/>
+      <c r="X1078" s="1"/>
+      <c r="Y1078" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="I41:M45"/>
+    <mergeCell ref="I46:M50"/>
+    <mergeCell ref="G52:K56"/>
+    <mergeCell ref="G57:K61"/>
+    <mergeCell ref="F67:K71"/>
+    <mergeCell ref="G72:L74"/>
+    <mergeCell ref="G75:L77"/>
+    <mergeCell ref="F91:K93"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Git: Unsorted modified files for indefinite cold storage
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="125">
   <si>
     <t>key</t>
   </si>
@@ -61,6 +61,15 @@
     <t>discordia/control</t>
   </si>
   <si>
+    <t>discordia/narrator-lobby</t>
+  </si>
+  <si>
+    <t>general/general-off-topic-discussions</t>
+  </si>
+  <si>
+    <t>general/botstuff-commands</t>
+  </si>
+  <si>
     <t>names</t>
   </si>
   <si>
@@ -106,6 +115,36 @@
     <t>NjgyNzkxNDAyNTY4Mjg2MjM5.XliJ-A.mW2tHnkgTiEDTsmwhy9odNkGYwA</t>
   </si>
   <si>
+    <t>StoryBot #6</t>
+  </si>
+  <si>
+    <t>Njg2ODkzOTY3OTc5MTg0Mjgz.Xmd2Ag.QoolieLSa06gDbuLaYvxFxC3HT4</t>
+  </si>
+  <si>
+    <t>StoryBot #7</t>
+  </si>
+  <si>
+    <t>Njg2ODk0OTMwNjk3NjUwMTky.Xmd6VQ.Yhv-NvPi-UhWnwu3hhfozKZ_9Cg</t>
+  </si>
+  <si>
+    <t>StoryBot #8</t>
+  </si>
+  <si>
+    <t>Njg2ODk1MTQwODc0MjIzNjk2.Xmd6YA.kaxYIS61dEPHf7lZDgYHNWWjyaQ</t>
+  </si>
+  <si>
+    <t>StoryBot #9</t>
+  </si>
+  <si>
+    <t>Njg2ODk1MzU5NDc3Mjg0ODg0.Xmd6aQ.ks5OetIMTW-pPLDP5ORqRaYniQ4</t>
+  </si>
+  <si>
+    <t>StoryBot #10</t>
+  </si>
+  <si>
+    <t>Njg2ODk1NTM3MzQxMjAyNDMy.Xmd6cQ.NWFjExc2S4XpfiinD26LfYKw1Po</t>
+  </si>
+  <si>
     <t>story bot timeout</t>
   </si>
   <si>
@@ -118,6 +157,12 @@
     <t>7s</t>
   </si>
   <si>
+    <t>story bot min typing interval</t>
+  </si>
+  <si>
+    <t>1.5s</t>
+  </si>
+  <si>
     <t>story channel timestep</t>
   </si>
   <si>
@@ -127,7 +172,7 @@
     <t>story reply selection delay</t>
   </si>
   <si>
-    <t>1.5s</t>
+    <t>2s</t>
   </si>
   <si>
     <t>upload acknowledge message</t>
@@ -177,15 +222,27 @@
     <t>upload success message</t>
   </si>
   <si>
-    <t>%(sender) Cool!, I've looked at your story and I think its... o.. k.... To play, ping me with this story code:
+    <t>80FF7F</t>
+  </si>
+  <si>
+    <t>%(sender) Cool!, I've looked at your story and I think its... o.. k.... To play, ping me in #narrator-lobby with this story code:
 ```
 @Narrator %(code)
 ```</t>
   </si>
   <si>
-    <t>%(sender) That... was... amazing!, I'm sure others would agree too!. To play, ping me with this story code:
+    <t>%(sender) That... was... amazing!, I'm sure others would agree too!. To play, ping me in #narrator-lobby with this story code:
 ```
 @Narrator %(code)
+```</t>
+  </si>
+  <si>
+    <t>upload privately message</t>
+  </si>
+  <si>
+    <t>%(sender) If you want to upload a story, you have to send that link to me **privately in DMs**.
+```
+@Narrator &lt;google sheet link&gt;
 ```</t>
   </si>
   <si>
@@ -198,13 +255,22 @@
     <t>Are you okay %(sender)?, There is no Story #%(code) !</t>
   </si>
   <si>
-    <t>intro</t>
+    <t>ending message</t>
+  </si>
+  <si>
+    <t>embed</t>
+  </si>
+  <si>
+    <t>%(message)</t>
   </si>
   <si>
     <t>title</t>
   </si>
   <si>
-    <t>`%(title)`</t>
+    <t>`%(title) (Story #%(id))`</t>
+  </si>
+  <si>
+    <t>intro</t>
   </si>
   <si>
     <t>description</t>
@@ -235,7 +301,7 @@
     <t>preparing</t>
   </si>
   <si>
-    <t>%(:yes:) Getting ready...</t>
+    <t>%(:yes:) Getting ready... please wait.</t>
   </si>
   <si>
     <t>not enough resources</t>
@@ -247,7 +313,7 @@
     <t>starting</t>
   </si>
   <si>
-    <t>%(:yes:) Starting now...</t>
+    <t>%(:yes:) Starting now..., to quit type `@Narrator quit`</t>
   </si>
   <si>
     <t>waiting color</t>
@@ -265,9 +331,6 @@
     <t>starting color</t>
   </si>
   <si>
-    <t>80FF7F</t>
-  </si>
-  <si>
     <t>intro invite timeout</t>
   </si>
   <si>
@@ -283,11 +346,56 @@
     <t>instance timeout</t>
   </si>
   <si>
+    <t>instance speed command</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>instance quit command</t>
+  </si>
+  <si>
+    <t>quit</t>
+  </si>
+  <si>
+    <t>instance quit message</t>
+  </si>
+  <si>
+    <t>%(participant) wants to quit. Story will end in 60 seconds if nothing happens.</t>
+  </si>
+  <si>
+    <t>instance quit failed message</t>
+  </si>
+  <si>
+    <t>%(participant) wants to quit. Cannot quit while story is progressing. Try later when everyone stops talking.</t>
+  </si>
+  <si>
+    <t>instance quit delay</t>
+  </si>
+  <si>
+    <t>60 sec</t>
+  </si>
+  <si>
     <t>choose reply message</t>
   </si>
   <si>
     <t>%(player) Choose your reply:
 %(selection)</t>
+  </si>
+  <si>
+    <t>choose reply and type message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%(player) **Type your response now: **
+Or choose a reply:
+%(selection)
+</t>
+  </si>
+  <si>
+    <t>choose reply type only message</t>
+  </si>
+  <si>
+    <t>%(player) **Type your response now**:</t>
   </si>
   <si>
     <t>choose reply row format</t>
@@ -923,7 +1031,9 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -948,14 +1058,12 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -981,7 +1089,9 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1006,13 +1116,9 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1037,10 +1143,14 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="D23" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="F23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="4"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1064,16 +1174,11 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1096,14 +1201,15 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="D25" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1128,12 +1234,9 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1156,13 +1259,15 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="D27" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1189,10 +1294,10 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1218,9 +1323,12 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="F29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -1243,15 +1351,14 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -1274,15 +1381,14 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1305,13 +1411,13 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1336,13 +1442,13 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1369,8 +1475,12 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="F34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1394,20 +1504,16 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="2" t="s">
+      <c r="F35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="G35" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I35" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1431,16 +1537,14 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="2" t="s">
-        <v>40</v>
+      <c r="F36" s="4" t="s">
+        <v>42</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I36" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1489,13 +1593,11 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="G38" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -1518,11 +1620,15 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
+      <c r="D39" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E39" s="1"/>
-      <c r="G39" s="4" t="s">
-        <v>46</v>
+      <c r="F39" s="4" t="s">
+        <v>45</v>
       </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -1545,9 +1651,14 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
+      <c r="D40" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
+      <c r="G40" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -1572,18 +1683,19 @@
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="G41" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I41" s="7" t="s">
+      <c r="F41" s="1"/>
+      <c r="G41" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -1601,10 +1713,20 @@
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="D42" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E42" s="1"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="4"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -1622,10 +1744,20 @@
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+      <c r="D43" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E43" s="1"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="4"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -1645,8 +1777,14 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="4"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -1664,10 +1802,24 @@
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="D45" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="E45" s="1"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="4"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
@@ -1687,15 +1839,20 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
       <c r="G46" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
-      <c r="I46" s="7" t="s">
-        <v>50</v>
+      <c r="I46" s="4" t="s">
+        <v>58</v>
       </c>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
@@ -1715,8 +1872,14 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="4"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
@@ -1734,10 +1897,18 @@
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
+      <c r="D48" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="E48" s="1"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="4"/>
+      <c r="G48" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
@@ -1757,8 +1928,14 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="4"/>
+      <c r="G49" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
@@ -1778,8 +1955,13 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="4"/>
+      <c r="F50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
@@ -1797,15 +1979,19 @@
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+      <c r="D51" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="E51" s="1"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
+      <c r="G51" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
@@ -1823,13 +2009,10 @@
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="G52" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="4"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
@@ -1849,7 +2032,8 @@
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="4"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
@@ -1869,7 +2053,8 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="4"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
@@ -1889,7 +2074,8 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="4"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
@@ -1909,7 +2095,15 @@
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+      <c r="G56" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
@@ -1929,10 +2123,8 @@
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="4"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
@@ -1952,7 +2144,8 @@
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="4"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
@@ -1972,7 +2165,8 @@
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="4"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
@@ -1992,7 +2186,8 @@
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="4"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
@@ -2012,7 +2207,13 @@
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
@@ -2030,13 +2231,19 @@
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
+      <c r="D62" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
+      <c r="G62" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
@@ -2054,23 +2261,10 @@
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="D63" s="2"/>
       <c r="E63" s="1"/>
-      <c r="G63" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H63" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
@@ -2088,21 +2282,10 @@
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
+      <c r="D64" s="2"/>
       <c r="E64" s="1"/>
-      <c r="G64" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
@@ -2120,13 +2303,10 @@
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
+      <c r="D65" s="2"/>
       <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
@@ -2144,22 +2324,10 @@
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="1"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
@@ -2177,15 +2345,17 @@
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="2" t="s">
-        <v>60</v>
+      <c r="D67" s="2"/>
+      <c r="E67" s="1"/>
+      <c r="G67" s="2" t="s">
+        <v>55</v>
       </c>
-      <c r="F67" s="7" t="s">
-        <v>61</v>
+      <c r="H67" s="6" t="s">
+        <v>67</v>
       </c>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
+      <c r="I67" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
@@ -2203,10 +2373,10 @@
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
+      <c r="D68" s="2"/>
       <c r="E68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
@@ -2224,10 +2394,10 @@
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="D69" s="2"/>
       <c r="E69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
@@ -2245,10 +2415,10 @@
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
+      <c r="D70" s="2"/>
       <c r="E70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
@@ -2266,10 +2436,10 @@
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
+      <c r="D71" s="2"/>
       <c r="E71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
@@ -2287,15 +2457,13 @@
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F72" s="2"/>
-      <c r="G72" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M72" s="1"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="1"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
@@ -2313,10 +2481,19 @@
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="M73" s="1"/>
+      <c r="D73" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E73" s="1"/>
+      <c r="G73" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
@@ -2334,10 +2511,10 @@
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="M74" s="1"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="1"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
@@ -2355,15 +2532,10 @@
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F75" s="2"/>
-      <c r="G75" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="M75" s="1"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="1"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
@@ -2381,10 +2553,10 @@
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="M76" s="1"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="1"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
@@ -2402,10 +2574,10 @@
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="M77" s="1"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="1"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
@@ -2423,22 +2595,13 @@
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="L78" s="1"/>
-      <c r="M78" s="1"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="1"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
@@ -2456,20 +2619,13 @@
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
+      <c r="D79" s="2"/>
       <c r="E79" s="1"/>
-      <c r="F79" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G79" s="1"/>
-      <c r="H79" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
-      <c r="M79" s="1"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
@@ -2487,16 +2643,19 @@
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G80" s="4" t="s">
+      <c r="D80" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="G80" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
@@ -2520,12 +2679,14 @@
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
-      <c r="F81" s="2" t="s">
-        <v>73</v>
+      <c r="G81" s="2" t="s">
+        <v>55</v>
       </c>
-      <c r="G81" s="1"/>
-      <c r="I81" s="6" t="s">
-        <v>41</v>
+      <c r="H81" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
@@ -2550,13 +2711,7 @@
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-      <c r="F82" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G82" s="1"/>
-      <c r="I82" s="6" t="s">
-        <v>75</v>
-      </c>
+      <c r="F82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
@@ -2578,14 +2733,18 @@
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
+      <c r="D83" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E83" s="1"/>
       <c r="F83" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G83" s="1"/>
-      <c r="I83" s="6" t="s">
-        <v>48</v>
+      <c r="G83" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
@@ -2610,12 +2769,12 @@
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-      <c r="F84" s="2" t="s">
-        <v>77</v>
+      <c r="F84" s="1"/>
+      <c r="G84" s="2" t="s">
+        <v>78</v>
       </c>
-      <c r="G84" s="1"/>
-      <c r="I84" s="6" t="s">
-        <v>78</v>
+      <c r="H84" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
@@ -2641,9 +2800,6 @@
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
@@ -2666,17 +2822,19 @@
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F86" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E86" s="1"/>
-      <c r="F86" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
-      <c r="I86" s="7"/>
-      <c r="J86" s="7"/>
-      <c r="K86" s="7"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
@@ -2696,18 +2854,13 @@
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="2" t="s">
+      <c r="D87" s="1"/>
+      <c r="E87" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E87" s="1"/>
       <c r="F87" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
-      <c r="I87" s="7"/>
-      <c r="J87" s="7"/>
-      <c r="K87" s="7"/>
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
@@ -2727,18 +2880,8 @@
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="D88" s="1"/>
       <c r="E88" s="1"/>
-      <c r="F88" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G88" s="7"/>
-      <c r="H88" s="7"/>
-      <c r="I88" s="7"/>
-      <c r="J88" s="7"/>
-      <c r="K88" s="7"/>
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
@@ -2758,14 +2901,8 @@
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="2"/>
+      <c r="D89" s="1"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
-      <c r="I89" s="7"/>
-      <c r="J89" s="7"/>
-      <c r="K89" s="7"/>
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
@@ -2785,14 +2922,8 @@
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="2"/>
+      <c r="D90" s="1"/>
       <c r="E90" s="1"/>
-      <c r="F90" s="7"/>
-      <c r="G90" s="7"/>
-      <c r="H90" s="7"/>
-      <c r="I90" s="7"/>
-      <c r="J90" s="7"/>
-      <c r="K90" s="7"/>
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
@@ -2812,13 +2943,8 @@
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="D91" s="1"/>
       <c r="E91" s="1"/>
-      <c r="F91" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
@@ -2839,8 +2965,13 @@
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="L92" s="1"/>
+      <c r="E92" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F92" s="2"/>
+      <c r="G92" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
@@ -2860,8 +2991,8 @@
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="L93" s="1"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
@@ -2880,19 +3011,9 @@
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E94" s="1"/>
-      <c r="F94" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="1"/>
-      <c r="J94" s="1"/>
-      <c r="K94" s="1"/>
-      <c r="L94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
@@ -2912,14 +3033,13 @@
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-      <c r="K95" s="1"/>
-      <c r="L95" s="1"/>
+      <c r="E95" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F95" s="2"/>
+      <c r="G95" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
@@ -2939,14 +3059,8 @@
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
-      <c r="J96" s="1"/>
-      <c r="K96" s="1"/>
-      <c r="L96" s="1"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
@@ -2966,14 +3080,8 @@
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
-      <c r="K97" s="1"/>
-      <c r="L97" s="1"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
@@ -2993,9 +3101,15 @@
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
+      <c r="E98" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
@@ -3021,9 +3135,13 @@
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
+      <c r="F99" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
+      <c r="H99" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
@@ -3048,8 +3166,12 @@
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
+      <c r="F100" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
@@ -3075,10 +3197,13 @@
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
+      <c r="F101" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
+      <c r="I101" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
@@ -3102,10 +3227,13 @@
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
+      <c r="F102" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
+      <c r="I102" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
@@ -3129,10 +3257,13 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
+      <c r="F103" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="I103" s="1"/>
+      <c r="I103" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
@@ -3156,10 +3287,13 @@
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
+      <c r="F104" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1"/>
+      <c r="I104" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
@@ -3208,14 +3342,18 @@
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
+      <c r="D106" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
-      <c r="H106" s="1"/>
-      <c r="I106" s="1"/>
-      <c r="J106" s="1"/>
-      <c r="K106" s="1"/>
+      <c r="F106" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G106" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7"/>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
@@ -3235,14 +3373,18 @@
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
+      <c r="D107" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="E107" s="1"/>
-      <c r="F107" s="1"/>
-      <c r="G107" s="1"/>
-      <c r="H107" s="1"/>
-      <c r="I107" s="1"/>
-      <c r="J107" s="1"/>
-      <c r="K107" s="1"/>
+      <c r="F107" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G107" s="7"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
@@ -3262,14 +3404,18 @@
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
+      <c r="D108" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
-      <c r="H108" s="1"/>
-      <c r="I108" s="1"/>
-      <c r="J108" s="1"/>
-      <c r="K108" s="1"/>
+      <c r="F108" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G108" s="7"/>
+      <c r="H108" s="7"/>
+      <c r="I108" s="7"/>
+      <c r="J108" s="7"/>
+      <c r="K108" s="7"/>
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
@@ -3289,14 +3435,14 @@
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
+      <c r="D109" s="2"/>
       <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="I109" s="1"/>
-      <c r="J109" s="1"/>
-      <c r="K109" s="1"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7"/>
+      <c r="H109" s="7"/>
+      <c r="I109" s="7"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
@@ -3313,21 +3459,21 @@
       <c r="Y109" s="1"/>
     </row>
     <row r="110">
-      <c r="A110" s="2" t="s">
-        <v>6</v>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="2" t="s">
+        <v>104</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>88</v>
+      <c r="E110" s="1"/>
+      <c r="F110" s="7" t="s">
+        <v>105</v>
       </c>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-      <c r="I110" s="1"/>
-      <c r="J110" s="1"/>
-      <c r="K110" s="1"/>
+      <c r="G110" s="7"/>
+      <c r="H110" s="7"/>
+      <c r="I110" s="7"/>
+      <c r="J110" s="7"/>
+      <c r="K110" s="7"/>
       <c r="L110" s="1"/>
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
@@ -3347,14 +3493,14 @@
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
-      <c r="D111" s="1"/>
+      <c r="D111" s="2"/>
       <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
-      <c r="G111" s="1"/>
-      <c r="H111" s="1"/>
-      <c r="I111" s="1"/>
-      <c r="J111" s="1"/>
-      <c r="K111" s="1"/>
+      <c r="F111" s="7"/>
+      <c r="G111" s="7"/>
+      <c r="H111" s="7"/>
+      <c r="I111" s="7"/>
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
       <c r="L111" s="1"/>
       <c r="M111" s="1"/>
       <c r="N111" s="1"/>
@@ -3371,25 +3517,21 @@
       <c r="Y111" s="1"/>
     </row>
     <row r="112">
-      <c r="A112" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B112" s="4">
-        <v>5000.0</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D112" s="5" t="s">
-        <v>90</v>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
-      <c r="G112" s="1"/>
-      <c r="H112" s="1"/>
-      <c r="I112" s="1"/>
-      <c r="J112" s="1"/>
-      <c r="K112" s="1"/>
+      <c r="F112" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G112" s="7"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="7"/>
+      <c r="J112" s="7"/>
+      <c r="K112" s="7"/>
       <c r="L112" s="1"/>
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
@@ -3409,14 +3551,21 @@
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
+      <c r="D113" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="E113" s="1"/>
-      <c r="F113" s="1"/>
-      <c r="G113" s="1"/>
-      <c r="H113" s="1"/>
-      <c r="I113" s="1"/>
-      <c r="J113" s="1"/>
-      <c r="K113" s="1"/>
+      <c r="G113" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H113" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I113" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J113" s="7"/>
+      <c r="K113" s="7"/>
       <c r="L113" s="1"/>
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
@@ -3436,14 +3585,21 @@
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
+      <c r="D114" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
-      <c r="H114" s="1"/>
-      <c r="I114" s="1"/>
-      <c r="J114" s="1"/>
-      <c r="K114" s="1"/>
+      <c r="G114" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H114" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I114" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J114" s="7"/>
+      <c r="K114" s="7"/>
       <c r="L114" s="1"/>
       <c r="M114" s="1"/>
       <c r="N114" s="1"/>
@@ -3463,14 +3619,14 @@
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
+      <c r="D115" s="2"/>
       <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="1"/>
-      <c r="J115" s="1"/>
-      <c r="K115" s="1"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
+      <c r="H115" s="7"/>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
       <c r="L115" s="1"/>
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
@@ -3490,14 +3646,18 @@
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
+      <c r="D116" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
-      <c r="G116" s="1"/>
-      <c r="H116" s="1"/>
-      <c r="I116" s="1"/>
-      <c r="J116" s="1"/>
-      <c r="K116" s="1"/>
+      <c r="F116" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G116" s="7"/>
+      <c r="H116" s="7"/>
+      <c r="I116" s="7"/>
+      <c r="J116" s="7"/>
+      <c r="K116" s="7"/>
       <c r="L116" s="1"/>
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
@@ -3517,14 +3677,14 @@
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
+      <c r="D117" s="2"/>
       <c r="E117" s="1"/>
-      <c r="F117" s="1"/>
-      <c r="G117" s="1"/>
-      <c r="H117" s="1"/>
-      <c r="I117" s="1"/>
-      <c r="J117" s="1"/>
-      <c r="K117" s="1"/>
+      <c r="F117" s="7"/>
+      <c r="G117" s="7"/>
+      <c r="H117" s="7"/>
+      <c r="I117" s="7"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
       <c r="L117" s="1"/>
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
@@ -3544,14 +3704,14 @@
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
+      <c r="D118" s="2"/>
       <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-      <c r="I118" s="1"/>
-      <c r="J118" s="1"/>
-      <c r="K118" s="1"/>
+      <c r="F118" s="7"/>
+      <c r="G118" s="7"/>
+      <c r="H118" s="7"/>
+      <c r="I118" s="7"/>
+      <c r="J118" s="7"/>
+      <c r="K118" s="7"/>
       <c r="L118" s="1"/>
       <c r="M118" s="1"/>
       <c r="N118" s="1"/>
@@ -3571,14 +3731,13 @@
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
+      <c r="D119" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="E119" s="1"/>
-      <c r="F119" s="1"/>
-      <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
-      <c r="I119" s="1"/>
-      <c r="J119" s="1"/>
-      <c r="K119" s="1"/>
+      <c r="F119" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="L119" s="1"/>
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
@@ -3600,12 +3759,6 @@
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
-      <c r="F120" s="1"/>
-      <c r="G120" s="1"/>
-      <c r="H120" s="1"/>
-      <c r="I120" s="1"/>
-      <c r="J120" s="1"/>
-      <c r="K120" s="1"/>
       <c r="L120" s="1"/>
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
@@ -3627,12 +3780,6 @@
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
-      <c r="G121" s="1"/>
-      <c r="H121" s="1"/>
-      <c r="I121" s="1"/>
-      <c r="J121" s="1"/>
-      <c r="K121" s="1"/>
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
       <c r="N121" s="1"/>
@@ -3652,15 +3799,13 @@
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
+      <c r="D122" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="E122" s="1"/>
-      <c r="F122" s="1"/>
-      <c r="G122" s="1"/>
-      <c r="H122" s="1"/>
-      <c r="I122" s="1"/>
-      <c r="J122" s="1"/>
-      <c r="K122" s="1"/>
-      <c r="L122" s="1"/>
+      <c r="G122" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="M122" s="1"/>
       <c r="N122" s="1"/>
       <c r="O122" s="1"/>
@@ -3681,13 +3826,6 @@
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
-      <c r="F123" s="1"/>
-      <c r="G123" s="1"/>
-      <c r="H123" s="1"/>
-      <c r="I123" s="1"/>
-      <c r="J123" s="1"/>
-      <c r="K123" s="1"/>
-      <c r="L123" s="1"/>
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
       <c r="O123" s="1"/>
@@ -3708,13 +3846,6 @@
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="1"/>
-      <c r="G124" s="1"/>
-      <c r="H124" s="1"/>
-      <c r="I124" s="1"/>
-      <c r="J124" s="1"/>
-      <c r="K124" s="1"/>
-      <c r="L124" s="1"/>
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
       <c r="O124" s="1"/>
@@ -3735,13 +3866,6 @@
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
-      <c r="F125" s="1"/>
-      <c r="G125" s="1"/>
-      <c r="H125" s="1"/>
-      <c r="I125" s="1"/>
-      <c r="J125" s="1"/>
-      <c r="K125" s="1"/>
-      <c r="L125" s="1"/>
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
       <c r="O125" s="1"/>
@@ -3762,13 +3886,6 @@
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
-      <c r="F126" s="1"/>
-      <c r="G126" s="1"/>
-      <c r="H126" s="1"/>
-      <c r="I126" s="1"/>
-      <c r="J126" s="1"/>
-      <c r="K126" s="1"/>
-      <c r="L126" s="1"/>
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
       <c r="O126" s="1"/>
@@ -3787,16 +3904,13 @@
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
-      <c r="D127" s="1"/>
+      <c r="D127" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="E127" s="1"/>
-      <c r="F127" s="1"/>
-      <c r="G127" s="1"/>
-      <c r="H127" s="1"/>
-      <c r="I127" s="1"/>
-      <c r="J127" s="1"/>
-      <c r="K127" s="1"/>
-      <c r="L127" s="1"/>
-      <c r="M127" s="1"/>
+      <c r="G127" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="N127" s="1"/>
       <c r="O127" s="1"/>
       <c r="P127" s="1"/>
@@ -3816,13 +3930,6 @@
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
-      <c r="F128" s="1"/>
-      <c r="G128" s="1"/>
-      <c r="H128" s="1"/>
-      <c r="I128" s="1"/>
-      <c r="J128" s="1"/>
-      <c r="K128" s="1"/>
-      <c r="L128" s="1"/>
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
       <c r="O128" s="1"/>
@@ -3841,9 +3948,13 @@
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
-      <c r="D129" s="1"/>
+      <c r="D129" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="E129" s="1"/>
-      <c r="F129" s="1"/>
+      <c r="F129" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
       <c r="I129" s="1"/>
@@ -4270,8 +4381,12 @@
       <c r="Y144" s="1"/>
     </row>
     <row r="145">
-      <c r="A145" s="1"/>
-      <c r="B145" s="1"/>
+      <c r="A145" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -4324,10 +4439,18 @@
       <c r="Y146" s="1"/>
     </row>
     <row r="147">
-      <c r="A147" s="1"/>
-      <c r="B147" s="1"/>
-      <c r="C147" s="1"/>
-      <c r="D147" s="1"/>
+      <c r="A147" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B147" s="4">
+        <v>5000.0</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
@@ -29487,16 +29610,964 @@
       <c r="X1078" s="1"/>
       <c r="Y1078" s="1"/>
     </row>
+    <row r="1079">
+      <c r="A1079" s="1"/>
+      <c r="B1079" s="1"/>
+      <c r="C1079" s="1"/>
+      <c r="D1079" s="1"/>
+      <c r="E1079" s="1"/>
+      <c r="F1079" s="1"/>
+      <c r="G1079" s="1"/>
+      <c r="H1079" s="1"/>
+      <c r="I1079" s="1"/>
+      <c r="J1079" s="1"/>
+      <c r="K1079" s="1"/>
+      <c r="L1079" s="1"/>
+      <c r="M1079" s="1"/>
+      <c r="N1079" s="1"/>
+      <c r="O1079" s="1"/>
+      <c r="P1079" s="1"/>
+      <c r="Q1079" s="1"/>
+      <c r="R1079" s="1"/>
+      <c r="S1079" s="1"/>
+      <c r="T1079" s="1"/>
+      <c r="U1079" s="1"/>
+      <c r="V1079" s="1"/>
+      <c r="W1079" s="1"/>
+      <c r="X1079" s="1"/>
+      <c r="Y1079" s="1"/>
+    </row>
+    <row r="1080">
+      <c r="A1080" s="1"/>
+      <c r="B1080" s="1"/>
+      <c r="C1080" s="1"/>
+      <c r="D1080" s="1"/>
+      <c r="E1080" s="1"/>
+      <c r="F1080" s="1"/>
+      <c r="G1080" s="1"/>
+      <c r="H1080" s="1"/>
+      <c r="I1080" s="1"/>
+      <c r="J1080" s="1"/>
+      <c r="K1080" s="1"/>
+      <c r="L1080" s="1"/>
+      <c r="M1080" s="1"/>
+      <c r="N1080" s="1"/>
+      <c r="O1080" s="1"/>
+      <c r="P1080" s="1"/>
+      <c r="Q1080" s="1"/>
+      <c r="R1080" s="1"/>
+      <c r="S1080" s="1"/>
+      <c r="T1080" s="1"/>
+      <c r="U1080" s="1"/>
+      <c r="V1080" s="1"/>
+      <c r="W1080" s="1"/>
+      <c r="X1080" s="1"/>
+      <c r="Y1080" s="1"/>
+    </row>
+    <row r="1081">
+      <c r="A1081" s="1"/>
+      <c r="B1081" s="1"/>
+      <c r="C1081" s="1"/>
+      <c r="D1081" s="1"/>
+      <c r="E1081" s="1"/>
+      <c r="F1081" s="1"/>
+      <c r="G1081" s="1"/>
+      <c r="H1081" s="1"/>
+      <c r="I1081" s="1"/>
+      <c r="J1081" s="1"/>
+      <c r="K1081" s="1"/>
+      <c r="L1081" s="1"/>
+      <c r="M1081" s="1"/>
+      <c r="N1081" s="1"/>
+      <c r="O1081" s="1"/>
+      <c r="P1081" s="1"/>
+      <c r="Q1081" s="1"/>
+      <c r="R1081" s="1"/>
+      <c r="S1081" s="1"/>
+      <c r="T1081" s="1"/>
+      <c r="U1081" s="1"/>
+      <c r="V1081" s="1"/>
+      <c r="W1081" s="1"/>
+      <c r="X1081" s="1"/>
+      <c r="Y1081" s="1"/>
+    </row>
+    <row r="1082">
+      <c r="A1082" s="1"/>
+      <c r="B1082" s="1"/>
+      <c r="C1082" s="1"/>
+      <c r="D1082" s="1"/>
+      <c r="E1082" s="1"/>
+      <c r="F1082" s="1"/>
+      <c r="G1082" s="1"/>
+      <c r="H1082" s="1"/>
+      <c r="I1082" s="1"/>
+      <c r="J1082" s="1"/>
+      <c r="K1082" s="1"/>
+      <c r="L1082" s="1"/>
+      <c r="M1082" s="1"/>
+      <c r="N1082" s="1"/>
+      <c r="O1082" s="1"/>
+      <c r="P1082" s="1"/>
+      <c r="Q1082" s="1"/>
+      <c r="R1082" s="1"/>
+      <c r="S1082" s="1"/>
+      <c r="T1082" s="1"/>
+      <c r="U1082" s="1"/>
+      <c r="V1082" s="1"/>
+      <c r="W1082" s="1"/>
+      <c r="X1082" s="1"/>
+      <c r="Y1082" s="1"/>
+    </row>
+    <row r="1083">
+      <c r="A1083" s="1"/>
+      <c r="B1083" s="1"/>
+      <c r="C1083" s="1"/>
+      <c r="D1083" s="1"/>
+      <c r="E1083" s="1"/>
+      <c r="F1083" s="1"/>
+      <c r="G1083" s="1"/>
+      <c r="H1083" s="1"/>
+      <c r="I1083" s="1"/>
+      <c r="J1083" s="1"/>
+      <c r="K1083" s="1"/>
+      <c r="L1083" s="1"/>
+      <c r="M1083" s="1"/>
+      <c r="N1083" s="1"/>
+      <c r="O1083" s="1"/>
+      <c r="P1083" s="1"/>
+      <c r="Q1083" s="1"/>
+      <c r="R1083" s="1"/>
+      <c r="S1083" s="1"/>
+      <c r="T1083" s="1"/>
+      <c r="U1083" s="1"/>
+      <c r="V1083" s="1"/>
+      <c r="W1083" s="1"/>
+      <c r="X1083" s="1"/>
+      <c r="Y1083" s="1"/>
+    </row>
+    <row r="1084">
+      <c r="A1084" s="1"/>
+      <c r="B1084" s="1"/>
+      <c r="C1084" s="1"/>
+      <c r="D1084" s="1"/>
+      <c r="E1084" s="1"/>
+      <c r="F1084" s="1"/>
+      <c r="G1084" s="1"/>
+      <c r="H1084" s="1"/>
+      <c r="I1084" s="1"/>
+      <c r="J1084" s="1"/>
+      <c r="K1084" s="1"/>
+      <c r="L1084" s="1"/>
+      <c r="M1084" s="1"/>
+      <c r="N1084" s="1"/>
+      <c r="O1084" s="1"/>
+      <c r="P1084" s="1"/>
+      <c r="Q1084" s="1"/>
+      <c r="R1084" s="1"/>
+      <c r="S1084" s="1"/>
+      <c r="T1084" s="1"/>
+      <c r="U1084" s="1"/>
+      <c r="V1084" s="1"/>
+      <c r="W1084" s="1"/>
+      <c r="X1084" s="1"/>
+      <c r="Y1084" s="1"/>
+    </row>
+    <row r="1085">
+      <c r="A1085" s="1"/>
+      <c r="B1085" s="1"/>
+      <c r="C1085" s="1"/>
+      <c r="D1085" s="1"/>
+      <c r="E1085" s="1"/>
+      <c r="F1085" s="1"/>
+      <c r="G1085" s="1"/>
+      <c r="H1085" s="1"/>
+      <c r="I1085" s="1"/>
+      <c r="J1085" s="1"/>
+      <c r="K1085" s="1"/>
+      <c r="L1085" s="1"/>
+      <c r="M1085" s="1"/>
+      <c r="N1085" s="1"/>
+      <c r="O1085" s="1"/>
+      <c r="P1085" s="1"/>
+      <c r="Q1085" s="1"/>
+      <c r="R1085" s="1"/>
+      <c r="S1085" s="1"/>
+      <c r="T1085" s="1"/>
+      <c r="U1085" s="1"/>
+      <c r="V1085" s="1"/>
+      <c r="W1085" s="1"/>
+      <c r="X1085" s="1"/>
+      <c r="Y1085" s="1"/>
+    </row>
+    <row r="1086">
+      <c r="A1086" s="1"/>
+      <c r="B1086" s="1"/>
+      <c r="C1086" s="1"/>
+      <c r="D1086" s="1"/>
+      <c r="E1086" s="1"/>
+      <c r="F1086" s="1"/>
+      <c r="G1086" s="1"/>
+      <c r="H1086" s="1"/>
+      <c r="I1086" s="1"/>
+      <c r="J1086" s="1"/>
+      <c r="K1086" s="1"/>
+      <c r="L1086" s="1"/>
+      <c r="M1086" s="1"/>
+      <c r="N1086" s="1"/>
+      <c r="O1086" s="1"/>
+      <c r="P1086" s="1"/>
+      <c r="Q1086" s="1"/>
+      <c r="R1086" s="1"/>
+      <c r="S1086" s="1"/>
+      <c r="T1086" s="1"/>
+      <c r="U1086" s="1"/>
+      <c r="V1086" s="1"/>
+      <c r="W1086" s="1"/>
+      <c r="X1086" s="1"/>
+      <c r="Y1086" s="1"/>
+    </row>
+    <row r="1087">
+      <c r="A1087" s="1"/>
+      <c r="B1087" s="1"/>
+      <c r="C1087" s="1"/>
+      <c r="D1087" s="1"/>
+      <c r="E1087" s="1"/>
+      <c r="F1087" s="1"/>
+      <c r="G1087" s="1"/>
+      <c r="H1087" s="1"/>
+      <c r="I1087" s="1"/>
+      <c r="J1087" s="1"/>
+      <c r="K1087" s="1"/>
+      <c r="L1087" s="1"/>
+      <c r="M1087" s="1"/>
+      <c r="N1087" s="1"/>
+      <c r="O1087" s="1"/>
+      <c r="P1087" s="1"/>
+      <c r="Q1087" s="1"/>
+      <c r="R1087" s="1"/>
+      <c r="S1087" s="1"/>
+      <c r="T1087" s="1"/>
+      <c r="U1087" s="1"/>
+      <c r="V1087" s="1"/>
+      <c r="W1087" s="1"/>
+      <c r="X1087" s="1"/>
+      <c r="Y1087" s="1"/>
+    </row>
+    <row r="1088">
+      <c r="A1088" s="1"/>
+      <c r="B1088" s="1"/>
+      <c r="C1088" s="1"/>
+      <c r="D1088" s="1"/>
+      <c r="E1088" s="1"/>
+      <c r="F1088" s="1"/>
+      <c r="G1088" s="1"/>
+      <c r="H1088" s="1"/>
+      <c r="I1088" s="1"/>
+      <c r="J1088" s="1"/>
+      <c r="K1088" s="1"/>
+      <c r="L1088" s="1"/>
+      <c r="M1088" s="1"/>
+      <c r="N1088" s="1"/>
+      <c r="O1088" s="1"/>
+      <c r="P1088" s="1"/>
+      <c r="Q1088" s="1"/>
+      <c r="R1088" s="1"/>
+      <c r="S1088" s="1"/>
+      <c r="T1088" s="1"/>
+      <c r="U1088" s="1"/>
+      <c r="V1088" s="1"/>
+      <c r="W1088" s="1"/>
+      <c r="X1088" s="1"/>
+      <c r="Y1088" s="1"/>
+    </row>
+    <row r="1089">
+      <c r="A1089" s="1"/>
+      <c r="B1089" s="1"/>
+      <c r="C1089" s="1"/>
+      <c r="D1089" s="1"/>
+      <c r="E1089" s="1"/>
+      <c r="F1089" s="1"/>
+      <c r="G1089" s="1"/>
+      <c r="H1089" s="1"/>
+      <c r="I1089" s="1"/>
+      <c r="J1089" s="1"/>
+      <c r="K1089" s="1"/>
+      <c r="L1089" s="1"/>
+      <c r="M1089" s="1"/>
+      <c r="N1089" s="1"/>
+      <c r="O1089" s="1"/>
+      <c r="P1089" s="1"/>
+      <c r="Q1089" s="1"/>
+      <c r="R1089" s="1"/>
+      <c r="S1089" s="1"/>
+      <c r="T1089" s="1"/>
+      <c r="U1089" s="1"/>
+      <c r="V1089" s="1"/>
+      <c r="W1089" s="1"/>
+      <c r="X1089" s="1"/>
+      <c r="Y1089" s="1"/>
+    </row>
+    <row r="1090">
+      <c r="A1090" s="1"/>
+      <c r="B1090" s="1"/>
+      <c r="C1090" s="1"/>
+      <c r="D1090" s="1"/>
+      <c r="E1090" s="1"/>
+      <c r="F1090" s="1"/>
+      <c r="G1090" s="1"/>
+      <c r="H1090" s="1"/>
+      <c r="I1090" s="1"/>
+      <c r="J1090" s="1"/>
+      <c r="K1090" s="1"/>
+      <c r="L1090" s="1"/>
+      <c r="M1090" s="1"/>
+      <c r="N1090" s="1"/>
+      <c r="O1090" s="1"/>
+      <c r="P1090" s="1"/>
+      <c r="Q1090" s="1"/>
+      <c r="R1090" s="1"/>
+      <c r="S1090" s="1"/>
+      <c r="T1090" s="1"/>
+      <c r="U1090" s="1"/>
+      <c r="V1090" s="1"/>
+      <c r="W1090" s="1"/>
+      <c r="X1090" s="1"/>
+      <c r="Y1090" s="1"/>
+    </row>
+    <row r="1091">
+      <c r="A1091" s="1"/>
+      <c r="B1091" s="1"/>
+      <c r="C1091" s="1"/>
+      <c r="D1091" s="1"/>
+      <c r="E1091" s="1"/>
+      <c r="F1091" s="1"/>
+      <c r="G1091" s="1"/>
+      <c r="H1091" s="1"/>
+      <c r="I1091" s="1"/>
+      <c r="J1091" s="1"/>
+      <c r="K1091" s="1"/>
+      <c r="L1091" s="1"/>
+      <c r="M1091" s="1"/>
+      <c r="N1091" s="1"/>
+      <c r="O1091" s="1"/>
+      <c r="P1091" s="1"/>
+      <c r="Q1091" s="1"/>
+      <c r="R1091" s="1"/>
+      <c r="S1091" s="1"/>
+      <c r="T1091" s="1"/>
+      <c r="U1091" s="1"/>
+      <c r="V1091" s="1"/>
+      <c r="W1091" s="1"/>
+      <c r="X1091" s="1"/>
+      <c r="Y1091" s="1"/>
+    </row>
+    <row r="1092">
+      <c r="A1092" s="1"/>
+      <c r="B1092" s="1"/>
+      <c r="C1092" s="1"/>
+      <c r="D1092" s="1"/>
+      <c r="E1092" s="1"/>
+      <c r="F1092" s="1"/>
+      <c r="G1092" s="1"/>
+      <c r="H1092" s="1"/>
+      <c r="I1092" s="1"/>
+      <c r="J1092" s="1"/>
+      <c r="K1092" s="1"/>
+      <c r="L1092" s="1"/>
+      <c r="M1092" s="1"/>
+      <c r="N1092" s="1"/>
+      <c r="O1092" s="1"/>
+      <c r="P1092" s="1"/>
+      <c r="Q1092" s="1"/>
+      <c r="R1092" s="1"/>
+      <c r="S1092" s="1"/>
+      <c r="T1092" s="1"/>
+      <c r="U1092" s="1"/>
+      <c r="V1092" s="1"/>
+      <c r="W1092" s="1"/>
+      <c r="X1092" s="1"/>
+      <c r="Y1092" s="1"/>
+    </row>
+    <row r="1093">
+      <c r="A1093" s="1"/>
+      <c r="B1093" s="1"/>
+      <c r="C1093" s="1"/>
+      <c r="D1093" s="1"/>
+      <c r="E1093" s="1"/>
+      <c r="F1093" s="1"/>
+      <c r="G1093" s="1"/>
+      <c r="H1093" s="1"/>
+      <c r="I1093" s="1"/>
+      <c r="J1093" s="1"/>
+      <c r="K1093" s="1"/>
+      <c r="L1093" s="1"/>
+      <c r="M1093" s="1"/>
+      <c r="N1093" s="1"/>
+      <c r="O1093" s="1"/>
+      <c r="P1093" s="1"/>
+      <c r="Q1093" s="1"/>
+      <c r="R1093" s="1"/>
+      <c r="S1093" s="1"/>
+      <c r="T1093" s="1"/>
+      <c r="U1093" s="1"/>
+      <c r="V1093" s="1"/>
+      <c r="W1093" s="1"/>
+      <c r="X1093" s="1"/>
+      <c r="Y1093" s="1"/>
+    </row>
+    <row r="1094">
+      <c r="A1094" s="1"/>
+      <c r="B1094" s="1"/>
+      <c r="C1094" s="1"/>
+      <c r="D1094" s="1"/>
+      <c r="E1094" s="1"/>
+      <c r="F1094" s="1"/>
+      <c r="G1094" s="1"/>
+      <c r="H1094" s="1"/>
+      <c r="I1094" s="1"/>
+      <c r="J1094" s="1"/>
+      <c r="K1094" s="1"/>
+      <c r="L1094" s="1"/>
+      <c r="M1094" s="1"/>
+      <c r="N1094" s="1"/>
+      <c r="O1094" s="1"/>
+      <c r="P1094" s="1"/>
+      <c r="Q1094" s="1"/>
+      <c r="R1094" s="1"/>
+      <c r="S1094" s="1"/>
+      <c r="T1094" s="1"/>
+      <c r="U1094" s="1"/>
+      <c r="V1094" s="1"/>
+      <c r="W1094" s="1"/>
+      <c r="X1094" s="1"/>
+      <c r="Y1094" s="1"/>
+    </row>
+    <row r="1095">
+      <c r="A1095" s="1"/>
+      <c r="B1095" s="1"/>
+      <c r="C1095" s="1"/>
+      <c r="D1095" s="1"/>
+      <c r="E1095" s="1"/>
+      <c r="F1095" s="1"/>
+      <c r="G1095" s="1"/>
+      <c r="H1095" s="1"/>
+      <c r="I1095" s="1"/>
+      <c r="J1095" s="1"/>
+      <c r="K1095" s="1"/>
+      <c r="L1095" s="1"/>
+      <c r="M1095" s="1"/>
+      <c r="N1095" s="1"/>
+      <c r="O1095" s="1"/>
+      <c r="P1095" s="1"/>
+      <c r="Q1095" s="1"/>
+      <c r="R1095" s="1"/>
+      <c r="S1095" s="1"/>
+      <c r="T1095" s="1"/>
+      <c r="U1095" s="1"/>
+      <c r="V1095" s="1"/>
+      <c r="W1095" s="1"/>
+      <c r="X1095" s="1"/>
+      <c r="Y1095" s="1"/>
+    </row>
+    <row r="1096">
+      <c r="A1096" s="1"/>
+      <c r="B1096" s="1"/>
+      <c r="C1096" s="1"/>
+      <c r="D1096" s="1"/>
+      <c r="E1096" s="1"/>
+      <c r="F1096" s="1"/>
+      <c r="G1096" s="1"/>
+      <c r="H1096" s="1"/>
+      <c r="I1096" s="1"/>
+      <c r="J1096" s="1"/>
+      <c r="K1096" s="1"/>
+      <c r="L1096" s="1"/>
+      <c r="M1096" s="1"/>
+      <c r="N1096" s="1"/>
+      <c r="O1096" s="1"/>
+      <c r="P1096" s="1"/>
+      <c r="Q1096" s="1"/>
+      <c r="R1096" s="1"/>
+      <c r="S1096" s="1"/>
+      <c r="T1096" s="1"/>
+      <c r="U1096" s="1"/>
+      <c r="V1096" s="1"/>
+      <c r="W1096" s="1"/>
+      <c r="X1096" s="1"/>
+      <c r="Y1096" s="1"/>
+    </row>
+    <row r="1097">
+      <c r="A1097" s="1"/>
+      <c r="B1097" s="1"/>
+      <c r="C1097" s="1"/>
+      <c r="D1097" s="1"/>
+      <c r="E1097" s="1"/>
+      <c r="F1097" s="1"/>
+      <c r="G1097" s="1"/>
+      <c r="H1097" s="1"/>
+      <c r="I1097" s="1"/>
+      <c r="J1097" s="1"/>
+      <c r="K1097" s="1"/>
+      <c r="L1097" s="1"/>
+      <c r="M1097" s="1"/>
+      <c r="N1097" s="1"/>
+      <c r="O1097" s="1"/>
+      <c r="P1097" s="1"/>
+      <c r="Q1097" s="1"/>
+      <c r="R1097" s="1"/>
+      <c r="S1097" s="1"/>
+      <c r="T1097" s="1"/>
+      <c r="U1097" s="1"/>
+      <c r="V1097" s="1"/>
+      <c r="W1097" s="1"/>
+      <c r="X1097" s="1"/>
+      <c r="Y1097" s="1"/>
+    </row>
+    <row r="1098">
+      <c r="A1098" s="1"/>
+      <c r="B1098" s="1"/>
+      <c r="C1098" s="1"/>
+      <c r="D1098" s="1"/>
+      <c r="E1098" s="1"/>
+      <c r="F1098" s="1"/>
+      <c r="G1098" s="1"/>
+      <c r="H1098" s="1"/>
+      <c r="I1098" s="1"/>
+      <c r="J1098" s="1"/>
+      <c r="K1098" s="1"/>
+      <c r="L1098" s="1"/>
+      <c r="M1098" s="1"/>
+      <c r="N1098" s="1"/>
+      <c r="O1098" s="1"/>
+      <c r="P1098" s="1"/>
+      <c r="Q1098" s="1"/>
+      <c r="R1098" s="1"/>
+      <c r="S1098" s="1"/>
+      <c r="T1098" s="1"/>
+      <c r="U1098" s="1"/>
+      <c r="V1098" s="1"/>
+      <c r="W1098" s="1"/>
+      <c r="X1098" s="1"/>
+      <c r="Y1098" s="1"/>
+    </row>
+    <row r="1099">
+      <c r="A1099" s="1"/>
+      <c r="B1099" s="1"/>
+      <c r="C1099" s="1"/>
+      <c r="D1099" s="1"/>
+      <c r="E1099" s="1"/>
+      <c r="F1099" s="1"/>
+      <c r="G1099" s="1"/>
+      <c r="H1099" s="1"/>
+      <c r="I1099" s="1"/>
+      <c r="J1099" s="1"/>
+      <c r="K1099" s="1"/>
+      <c r="L1099" s="1"/>
+      <c r="M1099" s="1"/>
+      <c r="N1099" s="1"/>
+      <c r="O1099" s="1"/>
+      <c r="P1099" s="1"/>
+      <c r="Q1099" s="1"/>
+      <c r="R1099" s="1"/>
+      <c r="S1099" s="1"/>
+      <c r="T1099" s="1"/>
+      <c r="U1099" s="1"/>
+      <c r="V1099" s="1"/>
+      <c r="W1099" s="1"/>
+      <c r="X1099" s="1"/>
+      <c r="Y1099" s="1"/>
+    </row>
+    <row r="1100">
+      <c r="A1100" s="1"/>
+      <c r="B1100" s="1"/>
+      <c r="C1100" s="1"/>
+      <c r="D1100" s="1"/>
+      <c r="E1100" s="1"/>
+      <c r="F1100" s="1"/>
+      <c r="G1100" s="1"/>
+      <c r="H1100" s="1"/>
+      <c r="I1100" s="1"/>
+      <c r="J1100" s="1"/>
+      <c r="K1100" s="1"/>
+      <c r="L1100" s="1"/>
+      <c r="M1100" s="1"/>
+      <c r="N1100" s="1"/>
+      <c r="O1100" s="1"/>
+      <c r="P1100" s="1"/>
+      <c r="Q1100" s="1"/>
+      <c r="R1100" s="1"/>
+      <c r="S1100" s="1"/>
+      <c r="T1100" s="1"/>
+      <c r="U1100" s="1"/>
+      <c r="V1100" s="1"/>
+      <c r="W1100" s="1"/>
+      <c r="X1100" s="1"/>
+      <c r="Y1100" s="1"/>
+    </row>
+    <row r="1101">
+      <c r="A1101" s="1"/>
+      <c r="B1101" s="1"/>
+      <c r="C1101" s="1"/>
+      <c r="D1101" s="1"/>
+      <c r="E1101" s="1"/>
+      <c r="F1101" s="1"/>
+      <c r="G1101" s="1"/>
+      <c r="H1101" s="1"/>
+      <c r="I1101" s="1"/>
+      <c r="J1101" s="1"/>
+      <c r="K1101" s="1"/>
+      <c r="L1101" s="1"/>
+      <c r="M1101" s="1"/>
+      <c r="N1101" s="1"/>
+      <c r="O1101" s="1"/>
+      <c r="P1101" s="1"/>
+      <c r="Q1101" s="1"/>
+      <c r="R1101" s="1"/>
+      <c r="S1101" s="1"/>
+      <c r="T1101" s="1"/>
+      <c r="U1101" s="1"/>
+      <c r="V1101" s="1"/>
+      <c r="W1101" s="1"/>
+      <c r="X1101" s="1"/>
+      <c r="Y1101" s="1"/>
+    </row>
+    <row r="1102">
+      <c r="A1102" s="1"/>
+      <c r="B1102" s="1"/>
+      <c r="C1102" s="1"/>
+      <c r="D1102" s="1"/>
+      <c r="E1102" s="1"/>
+      <c r="F1102" s="1"/>
+      <c r="G1102" s="1"/>
+      <c r="H1102" s="1"/>
+      <c r="I1102" s="1"/>
+      <c r="J1102" s="1"/>
+      <c r="K1102" s="1"/>
+      <c r="L1102" s="1"/>
+      <c r="M1102" s="1"/>
+      <c r="N1102" s="1"/>
+      <c r="O1102" s="1"/>
+      <c r="P1102" s="1"/>
+      <c r="Q1102" s="1"/>
+      <c r="R1102" s="1"/>
+      <c r="S1102" s="1"/>
+      <c r="T1102" s="1"/>
+      <c r="U1102" s="1"/>
+      <c r="V1102" s="1"/>
+      <c r="W1102" s="1"/>
+      <c r="X1102" s="1"/>
+      <c r="Y1102" s="1"/>
+    </row>
+    <row r="1103">
+      <c r="A1103" s="1"/>
+      <c r="B1103" s="1"/>
+      <c r="C1103" s="1"/>
+      <c r="D1103" s="1"/>
+      <c r="E1103" s="1"/>
+      <c r="F1103" s="1"/>
+      <c r="G1103" s="1"/>
+      <c r="H1103" s="1"/>
+      <c r="I1103" s="1"/>
+      <c r="J1103" s="1"/>
+      <c r="K1103" s="1"/>
+      <c r="L1103" s="1"/>
+      <c r="M1103" s="1"/>
+      <c r="N1103" s="1"/>
+      <c r="O1103" s="1"/>
+      <c r="P1103" s="1"/>
+      <c r="Q1103" s="1"/>
+      <c r="R1103" s="1"/>
+      <c r="S1103" s="1"/>
+      <c r="T1103" s="1"/>
+      <c r="U1103" s="1"/>
+      <c r="V1103" s="1"/>
+      <c r="W1103" s="1"/>
+      <c r="X1103" s="1"/>
+      <c r="Y1103" s="1"/>
+    </row>
+    <row r="1104">
+      <c r="A1104" s="1"/>
+      <c r="B1104" s="1"/>
+      <c r="C1104" s="1"/>
+      <c r="D1104" s="1"/>
+      <c r="E1104" s="1"/>
+      <c r="F1104" s="1"/>
+      <c r="G1104" s="1"/>
+      <c r="H1104" s="1"/>
+      <c r="I1104" s="1"/>
+      <c r="J1104" s="1"/>
+      <c r="K1104" s="1"/>
+      <c r="L1104" s="1"/>
+      <c r="M1104" s="1"/>
+      <c r="N1104" s="1"/>
+      <c r="O1104" s="1"/>
+      <c r="P1104" s="1"/>
+      <c r="Q1104" s="1"/>
+      <c r="R1104" s="1"/>
+      <c r="S1104" s="1"/>
+      <c r="T1104" s="1"/>
+      <c r="U1104" s="1"/>
+      <c r="V1104" s="1"/>
+      <c r="W1104" s="1"/>
+      <c r="X1104" s="1"/>
+      <c r="Y1104" s="1"/>
+    </row>
+    <row r="1105">
+      <c r="A1105" s="1"/>
+      <c r="B1105" s="1"/>
+      <c r="C1105" s="1"/>
+      <c r="D1105" s="1"/>
+      <c r="E1105" s="1"/>
+      <c r="F1105" s="1"/>
+      <c r="G1105" s="1"/>
+      <c r="H1105" s="1"/>
+      <c r="I1105" s="1"/>
+      <c r="J1105" s="1"/>
+      <c r="K1105" s="1"/>
+      <c r="L1105" s="1"/>
+      <c r="M1105" s="1"/>
+      <c r="N1105" s="1"/>
+      <c r="O1105" s="1"/>
+      <c r="P1105" s="1"/>
+      <c r="Q1105" s="1"/>
+      <c r="R1105" s="1"/>
+      <c r="S1105" s="1"/>
+      <c r="T1105" s="1"/>
+      <c r="U1105" s="1"/>
+      <c r="V1105" s="1"/>
+      <c r="W1105" s="1"/>
+      <c r="X1105" s="1"/>
+      <c r="Y1105" s="1"/>
+    </row>
+    <row r="1106">
+      <c r="A1106" s="1"/>
+      <c r="B1106" s="1"/>
+      <c r="C1106" s="1"/>
+      <c r="D1106" s="1"/>
+      <c r="E1106" s="1"/>
+      <c r="F1106" s="1"/>
+      <c r="G1106" s="1"/>
+      <c r="H1106" s="1"/>
+      <c r="I1106" s="1"/>
+      <c r="J1106" s="1"/>
+      <c r="K1106" s="1"/>
+      <c r="L1106" s="1"/>
+      <c r="M1106" s="1"/>
+      <c r="N1106" s="1"/>
+      <c r="O1106" s="1"/>
+      <c r="P1106" s="1"/>
+      <c r="Q1106" s="1"/>
+      <c r="R1106" s="1"/>
+      <c r="S1106" s="1"/>
+      <c r="T1106" s="1"/>
+      <c r="U1106" s="1"/>
+      <c r="V1106" s="1"/>
+      <c r="W1106" s="1"/>
+      <c r="X1106" s="1"/>
+      <c r="Y1106" s="1"/>
+    </row>
+    <row r="1107">
+      <c r="A1107" s="1"/>
+      <c r="B1107" s="1"/>
+      <c r="C1107" s="1"/>
+      <c r="D1107" s="1"/>
+      <c r="E1107" s="1"/>
+      <c r="F1107" s="1"/>
+      <c r="G1107" s="1"/>
+      <c r="H1107" s="1"/>
+      <c r="I1107" s="1"/>
+      <c r="J1107" s="1"/>
+      <c r="K1107" s="1"/>
+      <c r="L1107" s="1"/>
+      <c r="M1107" s="1"/>
+      <c r="N1107" s="1"/>
+      <c r="O1107" s="1"/>
+      <c r="P1107" s="1"/>
+      <c r="Q1107" s="1"/>
+      <c r="R1107" s="1"/>
+      <c r="S1107" s="1"/>
+      <c r="T1107" s="1"/>
+      <c r="U1107" s="1"/>
+      <c r="V1107" s="1"/>
+      <c r="W1107" s="1"/>
+      <c r="X1107" s="1"/>
+      <c r="Y1107" s="1"/>
+    </row>
+    <row r="1108">
+      <c r="A1108" s="1"/>
+      <c r="B1108" s="1"/>
+      <c r="C1108" s="1"/>
+      <c r="D1108" s="1"/>
+      <c r="E1108" s="1"/>
+      <c r="F1108" s="1"/>
+      <c r="G1108" s="1"/>
+      <c r="H1108" s="1"/>
+      <c r="I1108" s="1"/>
+      <c r="J1108" s="1"/>
+      <c r="K1108" s="1"/>
+      <c r="L1108" s="1"/>
+      <c r="M1108" s="1"/>
+      <c r="N1108" s="1"/>
+      <c r="O1108" s="1"/>
+      <c r="P1108" s="1"/>
+      <c r="Q1108" s="1"/>
+      <c r="R1108" s="1"/>
+      <c r="S1108" s="1"/>
+      <c r="T1108" s="1"/>
+      <c r="U1108" s="1"/>
+      <c r="V1108" s="1"/>
+      <c r="W1108" s="1"/>
+      <c r="X1108" s="1"/>
+      <c r="Y1108" s="1"/>
+    </row>
+    <row r="1109">
+      <c r="A1109" s="1"/>
+      <c r="B1109" s="1"/>
+      <c r="C1109" s="1"/>
+      <c r="D1109" s="1"/>
+      <c r="E1109" s="1"/>
+      <c r="F1109" s="1"/>
+      <c r="G1109" s="1"/>
+      <c r="H1109" s="1"/>
+      <c r="I1109" s="1"/>
+      <c r="J1109" s="1"/>
+      <c r="K1109" s="1"/>
+      <c r="L1109" s="1"/>
+      <c r="M1109" s="1"/>
+      <c r="N1109" s="1"/>
+      <c r="O1109" s="1"/>
+      <c r="P1109" s="1"/>
+      <c r="Q1109" s="1"/>
+      <c r="R1109" s="1"/>
+      <c r="S1109" s="1"/>
+      <c r="T1109" s="1"/>
+      <c r="U1109" s="1"/>
+      <c r="V1109" s="1"/>
+      <c r="W1109" s="1"/>
+      <c r="X1109" s="1"/>
+      <c r="Y1109" s="1"/>
+    </row>
+    <row r="1110">
+      <c r="A1110" s="1"/>
+      <c r="B1110" s="1"/>
+      <c r="C1110" s="1"/>
+      <c r="D1110" s="1"/>
+      <c r="E1110" s="1"/>
+      <c r="F1110" s="1"/>
+      <c r="G1110" s="1"/>
+      <c r="H1110" s="1"/>
+      <c r="I1110" s="1"/>
+      <c r="J1110" s="1"/>
+      <c r="K1110" s="1"/>
+      <c r="L1110" s="1"/>
+      <c r="M1110" s="1"/>
+      <c r="N1110" s="1"/>
+      <c r="O1110" s="1"/>
+      <c r="P1110" s="1"/>
+      <c r="Q1110" s="1"/>
+      <c r="R1110" s="1"/>
+      <c r="S1110" s="1"/>
+      <c r="T1110" s="1"/>
+      <c r="U1110" s="1"/>
+      <c r="V1110" s="1"/>
+      <c r="W1110" s="1"/>
+      <c r="X1110" s="1"/>
+      <c r="Y1110" s="1"/>
+    </row>
+    <row r="1111">
+      <c r="A1111" s="1"/>
+      <c r="B1111" s="1"/>
+      <c r="C1111" s="1"/>
+      <c r="D1111" s="1"/>
+      <c r="E1111" s="1"/>
+      <c r="F1111" s="1"/>
+      <c r="G1111" s="1"/>
+      <c r="H1111" s="1"/>
+      <c r="I1111" s="1"/>
+      <c r="J1111" s="1"/>
+      <c r="K1111" s="1"/>
+      <c r="L1111" s="1"/>
+      <c r="M1111" s="1"/>
+      <c r="N1111" s="1"/>
+      <c r="O1111" s="1"/>
+      <c r="P1111" s="1"/>
+      <c r="Q1111" s="1"/>
+      <c r="R1111" s="1"/>
+      <c r="S1111" s="1"/>
+      <c r="T1111" s="1"/>
+      <c r="U1111" s="1"/>
+      <c r="V1111" s="1"/>
+      <c r="W1111" s="1"/>
+      <c r="X1111" s="1"/>
+      <c r="Y1111" s="1"/>
+    </row>
+    <row r="1112">
+      <c r="A1112" s="1"/>
+      <c r="B1112" s="1"/>
+      <c r="C1112" s="1"/>
+      <c r="D1112" s="1"/>
+      <c r="E1112" s="1"/>
+      <c r="F1112" s="1"/>
+      <c r="G1112" s="1"/>
+      <c r="H1112" s="1"/>
+      <c r="I1112" s="1"/>
+      <c r="J1112" s="1"/>
+      <c r="K1112" s="1"/>
+      <c r="L1112" s="1"/>
+      <c r="M1112" s="1"/>
+      <c r="N1112" s="1"/>
+      <c r="O1112" s="1"/>
+      <c r="P1112" s="1"/>
+      <c r="Q1112" s="1"/>
+      <c r="R1112" s="1"/>
+      <c r="S1112" s="1"/>
+      <c r="T1112" s="1"/>
+      <c r="U1112" s="1"/>
+      <c r="V1112" s="1"/>
+      <c r="W1112" s="1"/>
+      <c r="X1112" s="1"/>
+      <c r="Y1112" s="1"/>
+    </row>
+    <row r="1113">
+      <c r="A1113" s="1"/>
+      <c r="B1113" s="1"/>
+      <c r="C1113" s="1"/>
+      <c r="D1113" s="1"/>
+      <c r="E1113" s="1"/>
+      <c r="F1113" s="1"/>
+      <c r="G1113" s="1"/>
+      <c r="H1113" s="1"/>
+      <c r="I1113" s="1"/>
+      <c r="J1113" s="1"/>
+      <c r="K1113" s="1"/>
+      <c r="L1113" s="1"/>
+      <c r="M1113" s="1"/>
+      <c r="N1113" s="1"/>
+      <c r="O1113" s="1"/>
+      <c r="P1113" s="1"/>
+      <c r="Q1113" s="1"/>
+      <c r="R1113" s="1"/>
+      <c r="S1113" s="1"/>
+      <c r="T1113" s="1"/>
+      <c r="U1113" s="1"/>
+      <c r="V1113" s="1"/>
+      <c r="W1113" s="1"/>
+      <c r="X1113" s="1"/>
+      <c r="Y1113" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="I41:M45"/>
-    <mergeCell ref="I46:M50"/>
-    <mergeCell ref="G52:K56"/>
-    <mergeCell ref="G57:K61"/>
-    <mergeCell ref="F67:K71"/>
-    <mergeCell ref="G72:L74"/>
-    <mergeCell ref="G75:L77"/>
-    <mergeCell ref="F91:K93"/>
+  <mergeCells count="11">
+    <mergeCell ref="F119:K121"/>
+    <mergeCell ref="G122:L126"/>
+    <mergeCell ref="G127:L128"/>
+    <mergeCell ref="I62:M66"/>
+    <mergeCell ref="I67:M71"/>
+    <mergeCell ref="I51:M55"/>
+    <mergeCell ref="I56:M60"/>
+    <mergeCell ref="F87:K91"/>
+    <mergeCell ref="G92:L94"/>
+    <mergeCell ref="G95:L97"/>
+    <mergeCell ref="I73:M77"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>